<commit_message>
config report in excel js
</commit_message>
<xml_diff>
--- a/public/templates/report_templateV4.xlsx
+++ b/public/templates/report_templateV4.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\gpro1\MyFiles\QuisVar\quisvar_proyect_ft\public\templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jcastillo\Documents\QuisVar\quisvar_proyect_ft\public\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCECD004-F5E1-433D-BDB7-FA2D5FCF76D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C38E35CC-CB35-417B-8F59-621442E12167}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="482" firstSheet="1" activeTab="1" xr2:uid="{F98A2DB2-54A5-485C-A701-CE43CF6B2BAF}"/>
   </bookViews>
@@ -1705,7 +1705,7 @@
     <numFmt numFmtId="168" formatCode="_ &quot;S/.&quot;\ * #,##0.00_ ;_ &quot;S/.&quot;\ * \-#,##0.00_ ;_ &quot;S/.&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="169" formatCode="&quot;S/&quot;\ #,##0.00"/>
   </numFmts>
-  <fonts count="39" x14ac:knownFonts="1">
+  <fonts count="40" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1967,6 +1967,12 @@
       <name val="Century Gothic"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="4"/>
+      <name val="Century Gothic"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="11">
     <fill>
@@ -2030,7 +2036,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="82">
+  <borders count="81">
     <border>
       <left/>
       <right/>
@@ -2851,17 +2857,6 @@
       <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
@@ -3072,7 +3067,7 @@
     <xf numFmtId="43" fontId="14" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="14" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="342">
+  <cellXfs count="343">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -3587,40 +3582,37 @@
     <xf numFmtId="9" fontId="29" fillId="9" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="9" borderId="68" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="9" borderId="65" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="9" borderId="67" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="37" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="9" borderId="68" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="9" borderId="67" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="9" borderId="68" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="27" fillId="9" borderId="67" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="9" borderId="75" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="27" fillId="9" borderId="74" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="9" borderId="68" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="25" fillId="9" borderId="67" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="9" borderId="75" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="25" fillId="9" borderId="74" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="9" borderId="68" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="9" borderId="67" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="9" borderId="75" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="9" borderId="74" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="38" fillId="9" borderId="68" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="38" fillId="9" borderId="67" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="38" fillId="9" borderId="75" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="38" fillId="9" borderId="74" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="23" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -3644,16 +3636,16 @@
     <xf numFmtId="0" fontId="28" fillId="9" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="31" fillId="9" borderId="72" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="31" fillId="9" borderId="71" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="28" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="9" fontId="29" fillId="9" borderId="72" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="29" fillId="9" borderId="71" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="9" fontId="29" fillId="9" borderId="79" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="29" fillId="9" borderId="78" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="9" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3677,9 +3669,102 @@
     <xf numFmtId="9" fontId="29" fillId="9" borderId="18" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="21" fillId="9" borderId="70" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="10" borderId="73" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="10" borderId="66" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="33" fillId="10" borderId="73" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="169" fontId="33" fillId="9" borderId="74" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="21" fillId="9" borderId="71" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="28" fillId="9" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="58" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="54" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="59" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="60" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="7" fillId="0" borderId="61" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="7" fillId="0" borderId="59" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="7" fillId="0" borderId="62" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="57" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="55" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="56" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="7" fillId="0" borderId="60" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="19" fillId="9" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="19" fillId="9" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="9" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="9" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="164" fontId="19" fillId="9" borderId="32" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -3689,6 +3774,30 @@
     <xf numFmtId="164" fontId="19" fillId="9" borderId="31" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="19" fillId="9" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="9" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="9" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -3701,104 +3810,119 @@
     <xf numFmtId="0" fontId="12" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="9" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="58" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="35" fillId="9" borderId="67" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="9" borderId="74" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="169" fontId="35" fillId="10" borderId="74" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="169" fontId="35" fillId="10" borderId="73" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="54" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="36" fillId="9" borderId="67" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="36" fillId="9" borderId="74" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="9" borderId="67" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="9" borderId="74" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="169" fontId="26" fillId="10" borderId="74" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="169" fontId="26" fillId="10" borderId="73" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="10" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="10" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="10" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="10" borderId="76" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="10" borderId="72" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="10" borderId="67" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="10" borderId="74" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="10" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="10" borderId="79" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="10" borderId="80" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="10" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="10" borderId="74" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="9" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="10" borderId="73" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="9" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="9" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="9" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="19" fillId="9" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="19" fillId="9" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="7" fillId="0" borderId="61" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="7" fillId="0" borderId="59" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="7" fillId="0" borderId="60" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="7" fillId="0" borderId="62" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="59" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="60" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="57" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="55" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="56" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="21" fillId="10" borderId="65" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="10" borderId="66" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="9" borderId="74" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="9" borderId="73" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="10" borderId="74" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="10" borderId="73" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="10" borderId="65" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="10" borderId="66" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="9" borderId="67" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="9" borderId="74" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="10" borderId="75" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="10" borderId="68" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="10" borderId="77" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="23" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -3812,32 +3936,11 @@
     <xf numFmtId="0" fontId="24" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="9" borderId="75" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="9" borderId="74" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="10" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="35" fillId="9" borderId="68" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="9" borderId="75" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="36" fillId="9" borderId="68" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="36" fillId="9" borderId="75" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="9" borderId="68" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="9" borderId="75" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="23" fillId="10" borderId="69" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -3896,122 +3999,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="10" borderId="76" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="10" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="10" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="10" borderId="77" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="10" borderId="73" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="10" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="10" borderId="69" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="10" borderId="68" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="10" borderId="75" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="10" borderId="70" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="10" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="10" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="10" borderId="80" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="10" borderId="78" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="10" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="10" borderId="81" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="10" borderId="75" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="10" borderId="74" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="10" borderId="66" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="10" borderId="67" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="10" borderId="74" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="9" borderId="65" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="9" borderId="68" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="9" borderId="75" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="10" borderId="74" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="169" fontId="39" fillId="10" borderId="74" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="10" borderId="75" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="169" fontId="39" fillId="10" borderId="73" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="10" borderId="67" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="10" borderId="75" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="10" borderId="74" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="10" borderId="66" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="10" borderId="67" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="169" fontId="33" fillId="10" borderId="74" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="169" fontId="33" fillId="9" borderId="75" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="169" fontId="26" fillId="10" borderId="75" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="169" fontId="26" fillId="10" borderId="74" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="9" borderId="72" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="9" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="169" fontId="35" fillId="10" borderId="75" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="169" fontId="35" fillId="10" borderId="74" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -4374,174 +4372,174 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:56" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="246" t="s">
+      <c r="A1" s="270" t="s">
         <v>328</v>
       </c>
-      <c r="B1" s="245"/>
-      <c r="C1" s="245"/>
-      <c r="D1" s="245"/>
-      <c r="E1" s="245"/>
-      <c r="F1" s="245"/>
-      <c r="G1" s="245"/>
-      <c r="H1" s="245"/>
-      <c r="I1" s="245"/>
-      <c r="J1" s="245"/>
-      <c r="K1" s="245"/>
-      <c r="L1" s="245"/>
-      <c r="M1" s="245"/>
-      <c r="N1" s="245"/>
-      <c r="O1" s="244" t="s">
+      <c r="B1" s="269"/>
+      <c r="C1" s="269"/>
+      <c r="D1" s="269"/>
+      <c r="E1" s="269"/>
+      <c r="F1" s="269"/>
+      <c r="G1" s="269"/>
+      <c r="H1" s="269"/>
+      <c r="I1" s="269"/>
+      <c r="J1" s="269"/>
+      <c r="K1" s="269"/>
+      <c r="L1" s="269"/>
+      <c r="M1" s="269"/>
+      <c r="N1" s="269"/>
+      <c r="O1" s="268" t="s">
         <v>326</v>
       </c>
-      <c r="P1" s="244"/>
-      <c r="Q1" s="244"/>
-      <c r="R1" s="244"/>
-      <c r="S1" s="244"/>
-      <c r="T1" s="244"/>
-      <c r="U1" s="244"/>
-      <c r="V1" s="244"/>
-      <c r="W1" s="244"/>
-      <c r="X1" s="244"/>
-      <c r="Y1" s="244"/>
-      <c r="Z1" s="244"/>
-      <c r="AA1" s="244"/>
-      <c r="AB1" s="244"/>
-      <c r="AC1" s="244"/>
-      <c r="AD1" s="244"/>
-      <c r="AE1" s="244"/>
-      <c r="AF1" s="244"/>
-      <c r="AG1" s="244"/>
-      <c r="AH1" s="245" t="s">
+      <c r="P1" s="268"/>
+      <c r="Q1" s="268"/>
+      <c r="R1" s="268"/>
+      <c r="S1" s="268"/>
+      <c r="T1" s="268"/>
+      <c r="U1" s="268"/>
+      <c r="V1" s="268"/>
+      <c r="W1" s="268"/>
+      <c r="X1" s="268"/>
+      <c r="Y1" s="268"/>
+      <c r="Z1" s="268"/>
+      <c r="AA1" s="268"/>
+      <c r="AB1" s="268"/>
+      <c r="AC1" s="268"/>
+      <c r="AD1" s="268"/>
+      <c r="AE1" s="268"/>
+      <c r="AF1" s="268"/>
+      <c r="AG1" s="268"/>
+      <c r="AH1" s="269" t="s">
         <v>320</v>
       </c>
-      <c r="AI1" s="245"/>
-      <c r="AJ1" s="245"/>
-      <c r="AK1" s="245"/>
-      <c r="AL1" s="242" t="s">
+      <c r="AI1" s="269"/>
+      <c r="AJ1" s="269"/>
+      <c r="AK1" s="269"/>
+      <c r="AL1" s="266" t="s">
         <v>327</v>
       </c>
-      <c r="AM1" s="242"/>
-      <c r="AN1" s="242"/>
-      <c r="AO1" s="242"/>
-      <c r="AP1" s="242"/>
-      <c r="AQ1" s="242"/>
-      <c r="AR1" s="242"/>
-      <c r="AS1" s="242"/>
-      <c r="AT1" s="242"/>
-      <c r="AU1" s="242"/>
-      <c r="AV1" s="242"/>
-      <c r="AW1" s="242"/>
-      <c r="AX1" s="242"/>
-      <c r="AY1" s="242"/>
-      <c r="AZ1" s="242"/>
-      <c r="BA1" s="242"/>
-      <c r="BB1" s="242"/>
-      <c r="BC1" s="242"/>
-      <c r="BD1" s="243"/>
+      <c r="AM1" s="266"/>
+      <c r="AN1" s="266"/>
+      <c r="AO1" s="266"/>
+      <c r="AP1" s="266"/>
+      <c r="AQ1" s="266"/>
+      <c r="AR1" s="266"/>
+      <c r="AS1" s="266"/>
+      <c r="AT1" s="266"/>
+      <c r="AU1" s="266"/>
+      <c r="AV1" s="266"/>
+      <c r="AW1" s="266"/>
+      <c r="AX1" s="266"/>
+      <c r="AY1" s="266"/>
+      <c r="AZ1" s="266"/>
+      <c r="BA1" s="266"/>
+      <c r="BB1" s="266"/>
+      <c r="BC1" s="266"/>
+      <c r="BD1" s="267"/>
     </row>
     <row r="2" spans="1:56" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="265" t="s">
+      <c r="A2" s="236" t="s">
         <v>294</v>
       </c>
-      <c r="B2" s="266"/>
+      <c r="B2" s="237"/>
       <c r="C2" s="141" t="s">
         <v>287</v>
       </c>
-      <c r="D2" s="269" t="s">
+      <c r="D2" s="240" t="s">
         <v>330</v>
       </c>
-      <c r="E2" s="269"/>
-      <c r="F2" s="234" t="s">
+      <c r="E2" s="240"/>
+      <c r="F2" s="272" t="s">
         <v>329</v>
       </c>
-      <c r="G2" s="234"/>
-      <c r="H2" s="234"/>
-      <c r="I2" s="234"/>
-      <c r="J2" s="234"/>
-      <c r="K2" s="234"/>
-      <c r="L2" s="234"/>
-      <c r="M2" s="234"/>
-      <c r="N2" s="234"/>
-      <c r="O2" s="234"/>
-      <c r="P2" s="234"/>
-      <c r="Q2" s="234"/>
-      <c r="R2" s="234"/>
-      <c r="S2" s="234"/>
-      <c r="T2" s="234"/>
-      <c r="U2" s="234"/>
-      <c r="V2" s="234"/>
-      <c r="W2" s="234"/>
-      <c r="X2" s="234"/>
-      <c r="Y2" s="234"/>
-      <c r="Z2" s="234"/>
-      <c r="AA2" s="234"/>
-      <c r="AB2" s="234"/>
-      <c r="AC2" s="234"/>
-      <c r="AD2" s="234"/>
-      <c r="AE2" s="234"/>
-      <c r="AF2" s="234"/>
-      <c r="AG2" s="234"/>
-      <c r="AH2" s="234"/>
-      <c r="AI2" s="234"/>
-      <c r="AJ2" s="234"/>
-      <c r="AK2" s="234"/>
-      <c r="AL2" s="234"/>
-      <c r="AM2" s="234"/>
-      <c r="AN2" s="234"/>
-      <c r="AO2" s="234"/>
-      <c r="AP2" s="234"/>
-      <c r="AQ2" s="234"/>
-      <c r="AR2" s="234"/>
-      <c r="AS2" s="234"/>
-      <c r="AT2" s="234"/>
-      <c r="AU2" s="234"/>
-      <c r="AV2" s="234"/>
-      <c r="AW2" s="234"/>
-      <c r="AX2" s="234"/>
-      <c r="AY2" s="234"/>
-      <c r="AZ2" s="234"/>
-      <c r="BA2" s="234"/>
-      <c r="BB2" s="234"/>
-      <c r="BC2" s="234"/>
-      <c r="BD2" s="235"/>
+      <c r="G2" s="272"/>
+      <c r="H2" s="272"/>
+      <c r="I2" s="272"/>
+      <c r="J2" s="272"/>
+      <c r="K2" s="272"/>
+      <c r="L2" s="272"/>
+      <c r="M2" s="272"/>
+      <c r="N2" s="272"/>
+      <c r="O2" s="272"/>
+      <c r="P2" s="272"/>
+      <c r="Q2" s="272"/>
+      <c r="R2" s="272"/>
+      <c r="S2" s="272"/>
+      <c r="T2" s="272"/>
+      <c r="U2" s="272"/>
+      <c r="V2" s="272"/>
+      <c r="W2" s="272"/>
+      <c r="X2" s="272"/>
+      <c r="Y2" s="272"/>
+      <c r="Z2" s="272"/>
+      <c r="AA2" s="272"/>
+      <c r="AB2" s="272"/>
+      <c r="AC2" s="272"/>
+      <c r="AD2" s="272"/>
+      <c r="AE2" s="272"/>
+      <c r="AF2" s="272"/>
+      <c r="AG2" s="272"/>
+      <c r="AH2" s="272"/>
+      <c r="AI2" s="272"/>
+      <c r="AJ2" s="272"/>
+      <c r="AK2" s="272"/>
+      <c r="AL2" s="272"/>
+      <c r="AM2" s="272"/>
+      <c r="AN2" s="272"/>
+      <c r="AO2" s="272"/>
+      <c r="AP2" s="272"/>
+      <c r="AQ2" s="272"/>
+      <c r="AR2" s="272"/>
+      <c r="AS2" s="272"/>
+      <c r="AT2" s="272"/>
+      <c r="AU2" s="272"/>
+      <c r="AV2" s="272"/>
+      <c r="AW2" s="272"/>
+      <c r="AX2" s="272"/>
+      <c r="AY2" s="272"/>
+      <c r="AZ2" s="272"/>
+      <c r="BA2" s="272"/>
+      <c r="BB2" s="272"/>
+      <c r="BC2" s="272"/>
+      <c r="BD2" s="273"/>
     </row>
     <row r="3" spans="1:56" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="265" t="s">
+      <c r="A3" s="236" t="s">
         <v>295</v>
       </c>
-      <c r="B3" s="266"/>
+      <c r="B3" s="237"/>
       <c r="C3" s="141" t="s">
         <v>286</v>
       </c>
-      <c r="D3" s="248" t="s">
+      <c r="D3" s="265" t="s">
         <v>331</v>
       </c>
-      <c r="E3" s="248"/>
+      <c r="E3" s="265"/>
       <c r="F3" s="145">
         <v>75263586</v>
       </c>
       <c r="G3" s="145"/>
       <c r="H3" s="145"/>
-      <c r="I3" s="248" t="s">
+      <c r="I3" s="265" t="s">
         <v>335</v>
       </c>
-      <c r="J3" s="248"/>
-      <c r="K3" s="248"/>
-      <c r="L3" s="248"/>
-      <c r="M3" s="248"/>
-      <c r="N3" s="248"/>
-      <c r="O3" s="248"/>
-      <c r="P3" s="248"/>
-      <c r="Q3" s="248"/>
-      <c r="R3" s="237" t="s">
+      <c r="J3" s="265"/>
+      <c r="K3" s="265"/>
+      <c r="L3" s="265"/>
+      <c r="M3" s="265"/>
+      <c r="N3" s="265"/>
+      <c r="O3" s="265"/>
+      <c r="P3" s="265"/>
+      <c r="Q3" s="265"/>
+      <c r="R3" s="275" t="s">
         <v>337</v>
       </c>
-      <c r="S3" s="237"/>
-      <c r="T3" s="237"/>
-      <c r="U3" s="237"/>
-      <c r="V3" s="237"/>
-      <c r="W3" s="237"/>
-      <c r="X3" s="237"/>
+      <c r="S3" s="275"/>
+      <c r="T3" s="275"/>
+      <c r="U3" s="275"/>
+      <c r="V3" s="275"/>
+      <c r="W3" s="275"/>
+      <c r="X3" s="275"/>
       <c r="Y3" s="143"/>
       <c r="Z3" s="143"/>
       <c r="AA3" s="143"/>
@@ -4576,42 +4574,42 @@
       <c r="BD3" s="139"/>
     </row>
     <row r="4" spans="1:56" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="265" t="s">
+      <c r="A4" s="236" t="s">
         <v>296</v>
       </c>
-      <c r="B4" s="266"/>
+      <c r="B4" s="237"/>
       <c r="C4" s="141" t="s">
         <v>287</v>
       </c>
-      <c r="D4" s="248" t="s">
+      <c r="D4" s="265" t="s">
         <v>332</v>
       </c>
-      <c r="E4" s="248"/>
+      <c r="E4" s="265"/>
       <c r="F4" s="145">
         <v>99826036</v>
       </c>
       <c r="G4" s="145"/>
       <c r="H4" s="145"/>
-      <c r="I4" s="248" t="s">
+      <c r="I4" s="265" t="s">
         <v>336</v>
       </c>
-      <c r="J4" s="248"/>
-      <c r="K4" s="248"/>
-      <c r="L4" s="248"/>
-      <c r="M4" s="248"/>
-      <c r="N4" s="248"/>
-      <c r="O4" s="248"/>
-      <c r="P4" s="248"/>
-      <c r="Q4" s="248"/>
-      <c r="R4" s="237" t="s">
+      <c r="J4" s="265"/>
+      <c r="K4" s="265"/>
+      <c r="L4" s="265"/>
+      <c r="M4" s="265"/>
+      <c r="N4" s="265"/>
+      <c r="O4" s="265"/>
+      <c r="P4" s="265"/>
+      <c r="Q4" s="265"/>
+      <c r="R4" s="275" t="s">
         <v>338</v>
       </c>
-      <c r="S4" s="237"/>
-      <c r="T4" s="237"/>
-      <c r="U4" s="237"/>
-      <c r="V4" s="237"/>
-      <c r="W4" s="237"/>
-      <c r="X4" s="237"/>
+      <c r="S4" s="275"/>
+      <c r="T4" s="275"/>
+      <c r="U4" s="275"/>
+      <c r="V4" s="275"/>
+      <c r="W4" s="275"/>
+      <c r="X4" s="275"/>
       <c r="Y4" s="143"/>
       <c r="Z4" s="143"/>
       <c r="AA4" s="143"/>
@@ -4646,35 +4644,35 @@
       <c r="BD4" s="139"/>
     </row>
     <row r="5" spans="1:56" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="267" t="s">
+      <c r="A5" s="238" t="s">
         <v>302</v>
       </c>
-      <c r="B5" s="268"/>
+      <c r="B5" s="239"/>
       <c r="C5" s="142" t="s">
         <v>288</v>
       </c>
-      <c r="D5" s="270" t="s">
+      <c r="D5" s="241" t="s">
         <v>333</v>
       </c>
-      <c r="E5" s="270"/>
-      <c r="F5" s="236" t="s">
+      <c r="E5" s="241"/>
+      <c r="F5" s="274" t="s">
         <v>334</v>
       </c>
-      <c r="G5" s="236"/>
-      <c r="H5" s="236"/>
-      <c r="I5" s="236"/>
-      <c r="J5" s="236"/>
-      <c r="K5" s="236"/>
-      <c r="L5" s="236"/>
-      <c r="M5" s="236"/>
-      <c r="N5" s="236"/>
-      <c r="O5" s="236"/>
-      <c r="P5" s="236"/>
-      <c r="Q5" s="236"/>
-      <c r="R5" s="236"/>
-      <c r="S5" s="236"/>
-      <c r="T5" s="236"/>
-      <c r="U5" s="236"/>
+      <c r="G5" s="274"/>
+      <c r="H5" s="274"/>
+      <c r="I5" s="274"/>
+      <c r="J5" s="274"/>
+      <c r="K5" s="274"/>
+      <c r="L5" s="274"/>
+      <c r="M5" s="274"/>
+      <c r="N5" s="274"/>
+      <c r="O5" s="274"/>
+      <c r="P5" s="274"/>
+      <c r="Q5" s="274"/>
+      <c r="R5" s="274"/>
+      <c r="S5" s="274"/>
+      <c r="T5" s="274"/>
+      <c r="U5" s="274"/>
       <c r="V5" s="144"/>
       <c r="W5" s="144"/>
       <c r="X5" s="144"/>
@@ -4712,101 +4710,101 @@
       <c r="BD5" s="140"/>
     </row>
     <row r="6" spans="1:56" s="80" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="257" t="s">
+      <c r="A6" s="245" t="s">
         <v>313</v>
       </c>
-      <c r="B6" s="259" t="s">
+      <c r="B6" s="247" t="s">
         <v>160</v>
       </c>
-      <c r="C6" s="259" t="s">
+      <c r="C6" s="247" t="s">
         <v>157</v>
       </c>
-      <c r="D6" s="259" t="s">
+      <c r="D6" s="247" t="s">
         <v>292</v>
       </c>
-      <c r="E6" s="263" t="s">
+      <c r="E6" s="254" t="s">
         <v>159</v>
       </c>
-      <c r="F6" s="264"/>
-      <c r="G6" s="261" t="s">
+      <c r="F6" s="255"/>
+      <c r="G6" s="252" t="s">
         <v>293</v>
       </c>
-      <c r="H6" s="239" t="s">
+      <c r="H6" s="242" t="s">
         <v>135</v>
       </c>
-      <c r="I6" s="240"/>
-      <c r="J6" s="240"/>
-      <c r="K6" s="240"/>
-      <c r="L6" s="240"/>
-      <c r="M6" s="240"/>
-      <c r="N6" s="241"/>
-      <c r="O6" s="239" t="s">
+      <c r="I6" s="243"/>
+      <c r="J6" s="243"/>
+      <c r="K6" s="243"/>
+      <c r="L6" s="243"/>
+      <c r="M6" s="243"/>
+      <c r="N6" s="244"/>
+      <c r="O6" s="242" t="s">
         <v>136</v>
       </c>
-      <c r="P6" s="240"/>
-      <c r="Q6" s="240"/>
-      <c r="R6" s="240"/>
-      <c r="S6" s="240"/>
-      <c r="T6" s="240"/>
-      <c r="U6" s="241"/>
-      <c r="V6" s="239" t="s">
+      <c r="P6" s="243"/>
+      <c r="Q6" s="243"/>
+      <c r="R6" s="243"/>
+      <c r="S6" s="243"/>
+      <c r="T6" s="243"/>
+      <c r="U6" s="244"/>
+      <c r="V6" s="242" t="s">
         <v>1</v>
       </c>
-      <c r="W6" s="240"/>
-      <c r="X6" s="240"/>
-      <c r="Y6" s="240"/>
-      <c r="Z6" s="240"/>
-      <c r="AA6" s="240"/>
-      <c r="AB6" s="241"/>
-      <c r="AC6" s="239" t="s">
+      <c r="W6" s="243"/>
+      <c r="X6" s="243"/>
+      <c r="Y6" s="243"/>
+      <c r="Z6" s="243"/>
+      <c r="AA6" s="243"/>
+      <c r="AB6" s="244"/>
+      <c r="AC6" s="242" t="s">
         <v>137</v>
       </c>
-      <c r="AD6" s="240"/>
-      <c r="AE6" s="240"/>
-      <c r="AF6" s="240"/>
-      <c r="AG6" s="240"/>
-      <c r="AH6" s="240"/>
-      <c r="AI6" s="241"/>
-      <c r="AJ6" s="239" t="s">
+      <c r="AD6" s="243"/>
+      <c r="AE6" s="243"/>
+      <c r="AF6" s="243"/>
+      <c r="AG6" s="243"/>
+      <c r="AH6" s="243"/>
+      <c r="AI6" s="244"/>
+      <c r="AJ6" s="242" t="s">
         <v>84</v>
       </c>
-      <c r="AK6" s="240"/>
-      <c r="AL6" s="240"/>
-      <c r="AM6" s="240"/>
-      <c r="AN6" s="240"/>
-      <c r="AO6" s="240"/>
-      <c r="AP6" s="241"/>
-      <c r="AQ6" s="239" t="s">
+      <c r="AK6" s="243"/>
+      <c r="AL6" s="243"/>
+      <c r="AM6" s="243"/>
+      <c r="AN6" s="243"/>
+      <c r="AO6" s="243"/>
+      <c r="AP6" s="244"/>
+      <c r="AQ6" s="242" t="s">
         <v>138</v>
       </c>
-      <c r="AR6" s="240"/>
-      <c r="AS6" s="240"/>
-      <c r="AT6" s="240"/>
-      <c r="AU6" s="240"/>
-      <c r="AV6" s="240"/>
-      <c r="AW6" s="241"/>
-      <c r="AX6" s="239" t="s">
+      <c r="AR6" s="243"/>
+      <c r="AS6" s="243"/>
+      <c r="AT6" s="243"/>
+      <c r="AU6" s="243"/>
+      <c r="AV6" s="243"/>
+      <c r="AW6" s="244"/>
+      <c r="AX6" s="242" t="s">
         <v>139</v>
       </c>
-      <c r="AY6" s="240"/>
-      <c r="AZ6" s="240"/>
-      <c r="BA6" s="240"/>
-      <c r="BB6" s="240"/>
-      <c r="BC6" s="240"/>
-      <c r="BD6" s="241"/>
+      <c r="AY6" s="243"/>
+      <c r="AZ6" s="243"/>
+      <c r="BA6" s="243"/>
+      <c r="BB6" s="243"/>
+      <c r="BC6" s="243"/>
+      <c r="BD6" s="244"/>
     </row>
     <row r="7" spans="1:56" s="80" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="258"/>
-      <c r="B7" s="260"/>
-      <c r="C7" s="260"/>
-      <c r="D7" s="260"/>
+      <c r="A7" s="246"/>
+      <c r="B7" s="248"/>
+      <c r="C7" s="248"/>
+      <c r="D7" s="248"/>
       <c r="E7" s="154" t="s">
         <v>158</v>
       </c>
       <c r="F7" s="154" t="s">
         <v>312</v>
       </c>
-      <c r="G7" s="262"/>
+      <c r="G7" s="253"/>
       <c r="H7" s="155" t="s">
         <v>297</v>
       </c>
@@ -5080,7 +5078,7 @@
       <c r="BD9" s="89"/>
     </row>
     <row r="10" spans="1:56" s="80" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A10" s="253" t="s">
+      <c r="A10" s="249" t="s">
         <v>314</v>
       </c>
       <c r="B10" s="135"/>
@@ -5148,7 +5146,7 @@
       <c r="BD10" s="89"/>
     </row>
     <row r="11" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="254"/>
+      <c r="A11" s="250"/>
       <c r="B11" s="135"/>
       <c r="C11" s="90" t="s">
         <v>291</v>
@@ -5214,7 +5212,7 @@
       <c r="BD11" s="89"/>
     </row>
     <row r="12" spans="1:56" s="80" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A12" s="256"/>
+      <c r="A12" s="251"/>
       <c r="B12" s="135"/>
       <c r="C12" s="90" t="s">
         <v>89</v>
@@ -5404,7 +5402,7 @@
       <c r="BD14" s="89"/>
     </row>
     <row r="15" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="253" t="s">
+      <c r="A15" s="249" t="s">
         <v>315</v>
       </c>
       <c r="B15" s="135"/>
@@ -5474,7 +5472,7 @@
       <c r="BD15" s="89"/>
     </row>
     <row r="16" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="254"/>
+      <c r="A16" s="250"/>
       <c r="B16" s="135"/>
       <c r="C16" s="95" t="s">
         <v>104</v>
@@ -5542,7 +5540,7 @@
       <c r="BD16" s="89"/>
     </row>
     <row r="17" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="254"/>
+      <c r="A17" s="250"/>
       <c r="B17" s="135"/>
       <c r="C17" s="95" t="s">
         <v>105</v>
@@ -5610,7 +5608,7 @@
       <c r="BD17" s="89"/>
     </row>
     <row r="18" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="254"/>
+      <c r="A18" s="250"/>
       <c r="B18" s="135"/>
       <c r="C18" s="95" t="s">
         <v>106</v>
@@ -5678,7 +5676,7 @@
       <c r="BD18" s="89"/>
     </row>
     <row r="19" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="254"/>
+      <c r="A19" s="250"/>
       <c r="B19" s="135"/>
       <c r="C19" s="95" t="s">
         <v>99</v>
@@ -5746,7 +5744,7 @@
       <c r="BD19" s="89"/>
     </row>
     <row r="20" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="254"/>
+      <c r="A20" s="250"/>
       <c r="B20" s="135"/>
       <c r="C20" s="95" t="s">
         <v>107</v>
@@ -5814,7 +5812,7 @@
       <c r="BD20" s="89"/>
     </row>
     <row r="21" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="254"/>
+      <c r="A21" s="250"/>
       <c r="B21" s="135"/>
       <c r="C21" s="95" t="s">
         <v>108</v>
@@ -5882,7 +5880,7 @@
       <c r="BD21" s="89"/>
     </row>
     <row r="22" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="254"/>
+      <c r="A22" s="250"/>
       <c r="B22" s="135"/>
       <c r="C22" s="95" t="s">
         <v>109</v>
@@ -5950,7 +5948,7 @@
       <c r="BD22" s="89"/>
     </row>
     <row r="23" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="254"/>
+      <c r="A23" s="250"/>
       <c r="B23" s="135"/>
       <c r="C23" s="95" t="s">
         <v>110</v>
@@ -6018,7 +6016,7 @@
       <c r="BD23" s="89"/>
     </row>
     <row r="24" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="254"/>
+      <c r="A24" s="250"/>
       <c r="B24" s="135"/>
       <c r="C24" s="95" t="s">
         <v>111</v>
@@ -6086,7 +6084,7 @@
       <c r="BD24" s="89"/>
     </row>
     <row r="25" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="254"/>
+      <c r="A25" s="250"/>
       <c r="B25" s="135"/>
       <c r="C25" s="95" t="s">
         <v>112</v>
@@ -6154,7 +6152,7 @@
       <c r="BD25" s="89"/>
     </row>
     <row r="26" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="254"/>
+      <c r="A26" s="250"/>
       <c r="B26" s="135"/>
       <c r="C26" s="95" t="s">
         <v>113</v>
@@ -6222,7 +6220,7 @@
       <c r="BD26" s="89"/>
     </row>
     <row r="27" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="254"/>
+      <c r="A27" s="250"/>
       <c r="B27" s="135"/>
       <c r="C27" s="95" t="s">
         <v>114</v>
@@ -6290,7 +6288,7 @@
       <c r="BD27" s="89"/>
     </row>
     <row r="28" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="254"/>
+      <c r="A28" s="250"/>
       <c r="B28" s="135"/>
       <c r="C28" s="95" t="s">
         <v>115</v>
@@ -6358,7 +6356,7 @@
       <c r="BD28" s="89"/>
     </row>
     <row r="29" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="254"/>
+      <c r="A29" s="250"/>
       <c r="B29" s="135"/>
       <c r="C29" s="95" t="s">
         <v>116</v>
@@ -6426,7 +6424,7 @@
       <c r="BD29" s="89"/>
     </row>
     <row r="30" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="256"/>
+      <c r="A30" s="251"/>
       <c r="B30" s="135"/>
       <c r="C30" s="95" t="s">
         <v>117</v>
@@ -6556,7 +6554,7 @@
       <c r="BD31" s="89"/>
     </row>
     <row r="32" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="253" t="s">
+      <c r="A32" s="249" t="s">
         <v>316</v>
       </c>
       <c r="B32" s="135"/>
@@ -6624,7 +6622,7 @@
       <c r="BD32" s="89"/>
     </row>
     <row r="33" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="254"/>
+      <c r="A33" s="250"/>
       <c r="B33" s="135"/>
       <c r="C33" s="95" t="s">
         <v>105</v>
@@ -6690,7 +6688,7 @@
       <c r="BD33" s="89"/>
     </row>
     <row r="34" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="254"/>
+      <c r="A34" s="250"/>
       <c r="B34" s="135"/>
       <c r="C34" s="95" t="s">
         <v>108</v>
@@ -6756,7 +6754,7 @@
       <c r="BD34" s="89"/>
     </row>
     <row r="35" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="256"/>
+      <c r="A35" s="251"/>
       <c r="B35" s="135"/>
       <c r="C35" s="95" t="s">
         <v>91</v>
@@ -6884,7 +6882,7 @@
       <c r="BD36" s="89"/>
     </row>
     <row r="37" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="253" t="s">
+      <c r="A37" s="249" t="s">
         <v>317</v>
       </c>
       <c r="B37" s="136" t="s">
@@ -6948,7 +6946,7 @@
       <c r="BD37" s="89"/>
     </row>
     <row r="38" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="254"/>
+      <c r="A38" s="250"/>
       <c r="B38" s="137" t="s">
         <v>164</v>
       </c>
@@ -7016,7 +7014,7 @@
       <c r="BD38" s="89"/>
     </row>
     <row r="39" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="254"/>
+      <c r="A39" s="250"/>
       <c r="B39" s="137" t="s">
         <v>165</v>
       </c>
@@ -7084,7 +7082,7 @@
       <c r="BD39" s="89"/>
     </row>
     <row r="40" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="254"/>
+      <c r="A40" s="250"/>
       <c r="B40" s="136" t="s">
         <v>225</v>
       </c>
@@ -7146,7 +7144,7 @@
       <c r="BD40" s="89"/>
     </row>
     <row r="41" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="254"/>
+      <c r="A41" s="250"/>
       <c r="B41" s="137" t="s">
         <v>226</v>
       </c>
@@ -7214,7 +7212,7 @@
       <c r="BD41" s="89"/>
     </row>
     <row r="42" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="254"/>
+      <c r="A42" s="250"/>
       <c r="B42" s="136" t="s">
         <v>227</v>
       </c>
@@ -7276,7 +7274,7 @@
       <c r="BD42" s="89"/>
     </row>
     <row r="43" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="254"/>
+      <c r="A43" s="250"/>
       <c r="B43" s="137" t="s">
         <v>228</v>
       </c>
@@ -7340,7 +7338,7 @@
       <c r="BD43" s="89"/>
     </row>
     <row r="44" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="254"/>
+      <c r="A44" s="250"/>
       <c r="B44" s="135"/>
       <c r="C44" s="90" t="s">
         <v>174</v>
@@ -7406,7 +7404,7 @@
       <c r="BD44" s="89"/>
     </row>
     <row r="45" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="254"/>
+      <c r="A45" s="250"/>
       <c r="B45" s="135"/>
       <c r="C45" s="90" t="s">
         <v>173</v>
@@ -7472,7 +7470,7 @@
       <c r="BD45" s="89"/>
     </row>
     <row r="46" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="254"/>
+      <c r="A46" s="250"/>
       <c r="B46" s="136" t="s">
         <v>229</v>
       </c>
@@ -7534,7 +7532,7 @@
       <c r="BD46" s="89"/>
     </row>
     <row r="47" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="254"/>
+      <c r="A47" s="250"/>
       <c r="B47" s="137" t="s">
         <v>230</v>
       </c>
@@ -7602,7 +7600,7 @@
       <c r="BD47" s="89"/>
     </row>
     <row r="48" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="254"/>
+      <c r="A48" s="250"/>
       <c r="B48" s="137" t="s">
         <v>231</v>
       </c>
@@ -7670,7 +7668,7 @@
       <c r="BD48" s="89"/>
     </row>
     <row r="49" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="254"/>
+      <c r="A49" s="250"/>
       <c r="B49" s="137" t="s">
         <v>232</v>
       </c>
@@ -7738,7 +7736,7 @@
       <c r="BD49" s="89"/>
     </row>
     <row r="50" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="254"/>
+      <c r="A50" s="250"/>
       <c r="B50" s="137" t="s">
         <v>233</v>
       </c>
@@ -7806,7 +7804,7 @@
       <c r="BD50" s="89"/>
     </row>
     <row r="51" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="254"/>
+      <c r="A51" s="250"/>
       <c r="B51" s="136" t="s">
         <v>234</v>
       </c>
@@ -7868,7 +7866,7 @@
       <c r="BD51" s="89"/>
     </row>
     <row r="52" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="254"/>
+      <c r="A52" s="250"/>
       <c r="B52" s="137" t="s">
         <v>235</v>
       </c>
@@ -7936,7 +7934,7 @@
       <c r="BD52" s="89"/>
     </row>
     <row r="53" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="254"/>
+      <c r="A53" s="250"/>
       <c r="B53" s="137" t="s">
         <v>236</v>
       </c>
@@ -8004,7 +8002,7 @@
       <c r="BD53" s="89"/>
     </row>
     <row r="54" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="254"/>
+      <c r="A54" s="250"/>
       <c r="B54" s="136" t="s">
         <v>237</v>
       </c>
@@ -8066,7 +8064,7 @@
       <c r="BD54" s="89"/>
     </row>
     <row r="55" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="254"/>
+      <c r="A55" s="250"/>
       <c r="B55" s="137" t="s">
         <v>238</v>
       </c>
@@ -8132,7 +8130,7 @@
       <c r="BD55" s="89"/>
     </row>
     <row r="56" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="254"/>
+      <c r="A56" s="250"/>
       <c r="B56" s="135"/>
       <c r="C56" s="90" t="s">
         <v>183</v>
@@ -8200,7 +8198,7 @@
       <c r="BD56" s="89"/>
     </row>
     <row r="57" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="254"/>
+      <c r="A57" s="250"/>
       <c r="B57" s="135"/>
       <c r="C57" s="90" t="s">
         <v>182</v>
@@ -8268,7 +8266,7 @@
       <c r="BD57" s="89"/>
     </row>
     <row r="58" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="254"/>
+      <c r="A58" s="250"/>
       <c r="B58" s="137" t="s">
         <v>239</v>
       </c>
@@ -8334,7 +8332,7 @@
       <c r="BD58" s="89"/>
     </row>
     <row r="59" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="254"/>
+      <c r="A59" s="250"/>
       <c r="B59" s="135"/>
       <c r="C59" s="90" t="s">
         <v>282</v>
@@ -8402,7 +8400,7 @@
       <c r="BD59" s="89"/>
     </row>
     <row r="60" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="254"/>
+      <c r="A60" s="250"/>
       <c r="B60" s="135"/>
       <c r="C60" s="90" t="s">
         <v>283</v>
@@ -8470,7 +8468,7 @@
       <c r="BD60" s="89"/>
     </row>
     <row r="61" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="254"/>
+      <c r="A61" s="250"/>
       <c r="B61" s="136" t="s">
         <v>240</v>
       </c>
@@ -8532,7 +8530,7 @@
       <c r="BD61" s="89"/>
     </row>
     <row r="62" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="254"/>
+      <c r="A62" s="250"/>
       <c r="B62" s="137" t="s">
         <v>241</v>
       </c>
@@ -8600,7 +8598,7 @@
       <c r="BD62" s="89"/>
     </row>
     <row r="63" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="254"/>
+      <c r="A63" s="250"/>
       <c r="B63" s="137" t="s">
         <v>242</v>
       </c>
@@ -8668,7 +8666,7 @@
       <c r="BD63" s="89"/>
     </row>
     <row r="64" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="254"/>
+      <c r="A64" s="250"/>
       <c r="B64" s="136" t="s">
         <v>243</v>
       </c>
@@ -8730,7 +8728,7 @@
       <c r="BD64" s="89"/>
     </row>
     <row r="65" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="254"/>
+      <c r="A65" s="250"/>
       <c r="B65" s="137" t="s">
         <v>244</v>
       </c>
@@ -8798,7 +8796,7 @@
       <c r="BD65" s="89"/>
     </row>
     <row r="66" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="254"/>
+      <c r="A66" s="250"/>
       <c r="B66" s="136" t="s">
         <v>247</v>
       </c>
@@ -8860,7 +8858,7 @@
       <c r="BD66" s="89"/>
     </row>
     <row r="67" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="254"/>
+      <c r="A67" s="250"/>
       <c r="B67" s="137" t="s">
         <v>248</v>
       </c>
@@ -8928,7 +8926,7 @@
       <c r="BD67" s="89"/>
     </row>
     <row r="68" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="254"/>
+      <c r="A68" s="250"/>
       <c r="B68" s="136" t="s">
         <v>251</v>
       </c>
@@ -8990,7 +8988,7 @@
       <c r="BD68" s="89"/>
     </row>
     <row r="69" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="254"/>
+      <c r="A69" s="250"/>
       <c r="B69" s="137" t="s">
         <v>252</v>
       </c>
@@ -9058,7 +9056,7 @@
       <c r="BD69" s="89"/>
     </row>
     <row r="70" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="254"/>
+      <c r="A70" s="250"/>
       <c r="B70" s="137" t="s">
         <v>253</v>
       </c>
@@ -9126,7 +9124,7 @@
       <c r="BD70" s="89"/>
     </row>
     <row r="71" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="254"/>
+      <c r="A71" s="250"/>
       <c r="B71" s="136" t="s">
         <v>254</v>
       </c>
@@ -9188,7 +9186,7 @@
       <c r="BD71" s="89"/>
     </row>
     <row r="72" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="254"/>
+      <c r="A72" s="250"/>
       <c r="B72" s="137" t="s">
         <v>255</v>
       </c>
@@ -9256,7 +9254,7 @@
       <c r="BD72" s="89"/>
     </row>
     <row r="73" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="254"/>
+      <c r="A73" s="250"/>
       <c r="B73" s="136" t="s">
         <v>256</v>
       </c>
@@ -9318,7 +9316,7 @@
       <c r="BD73" s="89"/>
     </row>
     <row r="74" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="256"/>
+      <c r="A74" s="251"/>
       <c r="B74" s="137" t="s">
         <v>257</v>
       </c>
@@ -9510,7 +9508,7 @@
       <c r="BD76" s="89"/>
     </row>
     <row r="77" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A77" s="253" t="s">
+      <c r="A77" s="249" t="s">
         <v>162</v>
       </c>
       <c r="B77" s="135"/>
@@ -9578,7 +9576,7 @@
       <c r="BD77" s="89"/>
     </row>
     <row r="78" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A78" s="256"/>
+      <c r="A78" s="251"/>
       <c r="B78" s="135"/>
       <c r="C78" s="90" t="s">
         <v>95</v>
@@ -9706,7 +9704,7 @@
       <c r="BD79" s="89"/>
     </row>
     <row r="80" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A80" s="253" t="s">
+      <c r="A80" s="249" t="s">
         <v>162</v>
       </c>
       <c r="B80" s="135"/>
@@ -9774,7 +9772,7 @@
       <c r="BD80" s="89"/>
     </row>
     <row r="81" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A81" s="256"/>
+      <c r="A81" s="251"/>
       <c r="B81" s="135"/>
       <c r="C81" s="90" t="s">
         <v>93</v>
@@ -9902,7 +9900,7 @@
       <c r="BD82" s="89"/>
     </row>
     <row r="83" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A83" s="253" t="s">
+      <c r="A83" s="249" t="s">
         <v>162</v>
       </c>
       <c r="B83" s="135"/>
@@ -9970,7 +9968,7 @@
       <c r="BD83" s="89"/>
     </row>
     <row r="84" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A84" s="256"/>
+      <c r="A84" s="251"/>
       <c r="B84" s="135"/>
       <c r="C84" s="90" t="s">
         <v>134</v>
@@ -10160,7 +10158,7 @@
       <c r="BD86" s="89"/>
     </row>
     <row r="87" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A87" s="253" t="s">
+      <c r="A87" s="249" t="s">
         <v>319</v>
       </c>
       <c r="B87" s="135"/>
@@ -10228,7 +10226,7 @@
       <c r="BD87" s="89"/>
     </row>
     <row r="88" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A88" s="254"/>
+      <c r="A88" s="250"/>
       <c r="B88" s="135"/>
       <c r="C88" s="95" t="s">
         <v>119</v>
@@ -10294,7 +10292,7 @@
       <c r="BD88" s="89"/>
     </row>
     <row r="89" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A89" s="254"/>
+      <c r="A89" s="250"/>
       <c r="B89" s="135"/>
       <c r="C89" s="95" t="s">
         <v>120</v>
@@ -10360,7 +10358,7 @@
       <c r="BD89" s="89"/>
     </row>
     <row r="90" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A90" s="254"/>
+      <c r="A90" s="250"/>
       <c r="B90" s="135"/>
       <c r="C90" s="95" t="s">
         <v>121</v>
@@ -10426,7 +10424,7 @@
       <c r="BD90" s="89"/>
     </row>
     <row r="91" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A91" s="254"/>
+      <c r="A91" s="250"/>
       <c r="B91" s="135"/>
       <c r="C91" s="95" t="s">
         <v>122</v>
@@ -10492,7 +10490,7 @@
       <c r="BD91" s="89"/>
     </row>
     <row r="92" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A92" s="254"/>
+      <c r="A92" s="250"/>
       <c r="B92" s="135"/>
       <c r="C92" s="95" t="s">
         <v>123</v>
@@ -10558,7 +10556,7 @@
       <c r="BD92" s="89"/>
     </row>
     <row r="93" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A93" s="254"/>
+      <c r="A93" s="250"/>
       <c r="B93" s="135"/>
       <c r="C93" s="95" t="s">
         <v>124</v>
@@ -10624,7 +10622,7 @@
       <c r="BD93" s="89"/>
     </row>
     <row r="94" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A94" s="254"/>
+      <c r="A94" s="250"/>
       <c r="B94" s="135"/>
       <c r="C94" s="95" t="s">
         <v>125</v>
@@ -10690,7 +10688,7 @@
       <c r="BD94" s="89"/>
     </row>
     <row r="95" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A95" s="254"/>
+      <c r="A95" s="250"/>
       <c r="B95" s="135"/>
       <c r="C95" s="95" t="s">
         <v>126</v>
@@ -10756,7 +10754,7 @@
       <c r="BD95" s="89"/>
     </row>
     <row r="96" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A96" s="254"/>
+      <c r="A96" s="250"/>
       <c r="B96" s="135"/>
       <c r="C96" s="95" t="s">
         <v>127</v>
@@ -10822,7 +10820,7 @@
       <c r="BD96" s="89"/>
     </row>
     <row r="97" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A97" s="254"/>
+      <c r="A97" s="250"/>
       <c r="B97" s="135"/>
       <c r="C97" s="95" t="s">
         <v>128</v>
@@ -10888,7 +10886,7 @@
       <c r="BD97" s="89"/>
     </row>
     <row r="98" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A98" s="254"/>
+      <c r="A98" s="250"/>
       <c r="B98" s="135"/>
       <c r="C98" s="95" t="s">
         <v>129</v>
@@ -10954,7 +10952,7 @@
       <c r="BD98" s="89"/>
     </row>
     <row r="99" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A99" s="254"/>
+      <c r="A99" s="250"/>
       <c r="B99" s="135"/>
       <c r="C99" s="95" t="s">
         <v>130</v>
@@ -11020,7 +11018,7 @@
       <c r="BD99" s="89"/>
     </row>
     <row r="100" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A100" s="254"/>
+      <c r="A100" s="250"/>
       <c r="B100" s="135"/>
       <c r="C100" s="95" t="s">
         <v>131</v>
@@ -11086,7 +11084,7 @@
       <c r="BD100" s="89"/>
     </row>
     <row r="101" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A101" s="254"/>
+      <c r="A101" s="250"/>
       <c r="B101" s="135"/>
       <c r="C101" s="95" t="s">
         <v>132</v>
@@ -11152,7 +11150,7 @@
       <c r="BD101" s="89"/>
     </row>
     <row r="102" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A102" s="256"/>
+      <c r="A102" s="251"/>
       <c r="B102" s="135"/>
       <c r="C102" s="95" t="s">
         <v>133</v>
@@ -11280,7 +11278,7 @@
       <c r="BD103" s="89"/>
     </row>
     <row r="104" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A104" s="253" t="s">
+      <c r="A104" s="249" t="s">
         <v>318</v>
       </c>
       <c r="B104" s="136" t="s">
@@ -11344,7 +11342,7 @@
       <c r="BD104" s="89"/>
     </row>
     <row r="105" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A105" s="254"/>
+      <c r="A105" s="250"/>
       <c r="B105" s="137">
         <v>3.0101010000000001</v>
       </c>
@@ -11412,7 +11410,7 @@
       <c r="BD105" s="89"/>
     </row>
     <row r="106" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A106" s="254"/>
+      <c r="A106" s="250"/>
       <c r="B106" s="136" t="s">
         <v>224</v>
       </c>
@@ -11474,7 +11472,7 @@
       <c r="BD106" s="89"/>
     </row>
     <row r="107" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A107" s="254"/>
+      <c r="A107" s="250"/>
       <c r="B107" s="137" t="s">
         <v>164</v>
       </c>
@@ -11542,7 +11540,7 @@
       <c r="BD107" s="89"/>
     </row>
     <row r="108" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A108" s="254"/>
+      <c r="A108" s="250"/>
       <c r="B108" s="137" t="s">
         <v>165</v>
       </c>
@@ -11610,7 +11608,7 @@
       <c r="BD108" s="89"/>
     </row>
     <row r="109" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A109" s="254"/>
+      <c r="A109" s="250"/>
       <c r="B109" s="136" t="s">
         <v>225</v>
       </c>
@@ -11672,7 +11670,7 @@
       <c r="BD109" s="89"/>
     </row>
     <row r="110" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A110" s="254"/>
+      <c r="A110" s="250"/>
       <c r="B110" s="137" t="s">
         <v>226</v>
       </c>
@@ -11740,7 +11738,7 @@
       <c r="BD110" s="89"/>
     </row>
     <row r="111" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A111" s="254"/>
+      <c r="A111" s="250"/>
       <c r="B111" s="136" t="s">
         <v>227</v>
       </c>
@@ -11802,7 +11800,7 @@
       <c r="BD111" s="89"/>
     </row>
     <row r="112" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A112" s="254"/>
+      <c r="A112" s="250"/>
       <c r="B112" s="137" t="s">
         <v>228</v>
       </c>
@@ -11870,7 +11868,7 @@
       <c r="BD112" s="89"/>
     </row>
     <row r="113" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A113" s="254"/>
+      <c r="A113" s="250"/>
       <c r="B113" s="135"/>
       <c r="C113" s="90" t="s">
         <v>174</v>
@@ -11936,7 +11934,7 @@
       <c r="BD113" s="89"/>
     </row>
     <row r="114" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A114" s="254"/>
+      <c r="A114" s="250"/>
       <c r="B114" s="135"/>
       <c r="C114" s="90" t="s">
         <v>173</v>
@@ -12002,7 +12000,7 @@
       <c r="BD114" s="89"/>
     </row>
     <row r="115" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A115" s="254"/>
+      <c r="A115" s="250"/>
       <c r="B115" s="136" t="s">
         <v>229</v>
       </c>
@@ -12064,7 +12062,7 @@
       <c r="BD115" s="89"/>
     </row>
     <row r="116" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A116" s="254"/>
+      <c r="A116" s="250"/>
       <c r="B116" s="137" t="s">
         <v>230</v>
       </c>
@@ -12132,7 +12130,7 @@
       <c r="BD116" s="89"/>
     </row>
     <row r="117" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A117" s="254"/>
+      <c r="A117" s="250"/>
       <c r="B117" s="137" t="s">
         <v>231</v>
       </c>
@@ -12200,7 +12198,7 @@
       <c r="BD117" s="89"/>
     </row>
     <row r="118" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A118" s="254"/>
+      <c r="A118" s="250"/>
       <c r="B118" s="137" t="s">
         <v>232</v>
       </c>
@@ -12268,7 +12266,7 @@
       <c r="BD118" s="89"/>
     </row>
     <row r="119" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A119" s="254"/>
+      <c r="A119" s="250"/>
       <c r="B119" s="137" t="s">
         <v>233</v>
       </c>
@@ -12336,7 +12334,7 @@
       <c r="BD119" s="89"/>
     </row>
     <row r="120" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A120" s="254"/>
+      <c r="A120" s="250"/>
       <c r="B120" s="136" t="s">
         <v>234</v>
       </c>
@@ -12398,7 +12396,7 @@
       <c r="BD120" s="89"/>
     </row>
     <row r="121" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A121" s="254"/>
+      <c r="A121" s="250"/>
       <c r="B121" s="137" t="s">
         <v>235</v>
       </c>
@@ -12466,7 +12464,7 @@
       <c r="BD121" s="89"/>
     </row>
     <row r="122" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A122" s="254"/>
+      <c r="A122" s="250"/>
       <c r="B122" s="137" t="s">
         <v>236</v>
       </c>
@@ -12534,7 +12532,7 @@
       <c r="BD122" s="89"/>
     </row>
     <row r="123" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A123" s="254"/>
+      <c r="A123" s="250"/>
       <c r="B123" s="136" t="s">
         <v>237</v>
       </c>
@@ -12596,7 +12594,7 @@
       <c r="BD123" s="89"/>
     </row>
     <row r="124" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A124" s="254"/>
+      <c r="A124" s="250"/>
       <c r="B124" s="137" t="s">
         <v>238</v>
       </c>
@@ -12660,7 +12658,7 @@
       <c r="BD124" s="89"/>
     </row>
     <row r="125" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A125" s="254"/>
+      <c r="A125" s="250"/>
       <c r="B125" s="135"/>
       <c r="C125" s="90" t="s">
         <v>183</v>
@@ -12726,7 +12724,7 @@
       <c r="BD125" s="89"/>
     </row>
     <row r="126" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A126" s="254"/>
+      <c r="A126" s="250"/>
       <c r="B126" s="135"/>
       <c r="C126" s="90" t="s">
         <v>182</v>
@@ -12792,7 +12790,7 @@
       <c r="BD126" s="89"/>
     </row>
     <row r="127" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A127" s="254"/>
+      <c r="A127" s="250"/>
       <c r="B127" s="137" t="s">
         <v>239</v>
       </c>
@@ -12856,7 +12854,7 @@
       <c r="BD127" s="89"/>
     </row>
     <row r="128" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A128" s="254"/>
+      <c r="A128" s="250"/>
       <c r="B128" s="135"/>
       <c r="C128" s="90" t="s">
         <v>282</v>
@@ -12922,7 +12920,7 @@
       <c r="BD128" s="89"/>
     </row>
     <row r="129" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A129" s="254"/>
+      <c r="A129" s="250"/>
       <c r="B129" s="135"/>
       <c r="C129" s="90" t="s">
         <v>283</v>
@@ -12988,7 +12986,7 @@
       <c r="BD129" s="89"/>
     </row>
     <row r="130" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A130" s="254"/>
+      <c r="A130" s="250"/>
       <c r="B130" s="136" t="s">
         <v>240</v>
       </c>
@@ -13050,7 +13048,7 @@
       <c r="BD130" s="89"/>
     </row>
     <row r="131" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A131" s="254"/>
+      <c r="A131" s="250"/>
       <c r="B131" s="137" t="s">
         <v>241</v>
       </c>
@@ -13118,7 +13116,7 @@
       <c r="BD131" s="89"/>
     </row>
     <row r="132" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A132" s="254"/>
+      <c r="A132" s="250"/>
       <c r="B132" s="137" t="s">
         <v>242</v>
       </c>
@@ -13186,7 +13184,7 @@
       <c r="BD132" s="89"/>
     </row>
     <row r="133" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A133" s="254"/>
+      <c r="A133" s="250"/>
       <c r="B133" s="136" t="s">
         <v>243</v>
       </c>
@@ -13248,7 +13246,7 @@
       <c r="BD133" s="89"/>
     </row>
     <row r="134" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A134" s="254"/>
+      <c r="A134" s="250"/>
       <c r="B134" s="137" t="s">
         <v>244</v>
       </c>
@@ -13316,7 +13314,7 @@
       <c r="BD134" s="89"/>
     </row>
     <row r="135" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A135" s="254"/>
+      <c r="A135" s="250"/>
       <c r="B135" s="136" t="s">
         <v>247</v>
       </c>
@@ -13378,7 +13376,7 @@
       <c r="BD135" s="89"/>
     </row>
     <row r="136" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A136" s="254"/>
+      <c r="A136" s="250"/>
       <c r="B136" s="137" t="s">
         <v>248</v>
       </c>
@@ -13446,7 +13444,7 @@
       <c r="BD136" s="89"/>
     </row>
     <row r="137" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A137" s="254"/>
+      <c r="A137" s="250"/>
       <c r="B137" s="136" t="s">
         <v>249</v>
       </c>
@@ -13508,7 +13506,7 @@
       <c r="BD137" s="89"/>
     </row>
     <row r="138" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A138" s="254"/>
+      <c r="A138" s="250"/>
       <c r="B138" s="137" t="s">
         <v>250</v>
       </c>
@@ -13576,7 +13574,7 @@
       <c r="BD138" s="89"/>
     </row>
     <row r="139" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A139" s="254"/>
+      <c r="A139" s="250"/>
       <c r="B139" s="136" t="s">
         <v>251</v>
       </c>
@@ -13638,7 +13636,7 @@
       <c r="BD139" s="89"/>
     </row>
     <row r="140" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A140" s="254"/>
+      <c r="A140" s="250"/>
       <c r="B140" s="137" t="s">
         <v>252</v>
       </c>
@@ -13706,7 +13704,7 @@
       <c r="BD140" s="89"/>
     </row>
     <row r="141" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A141" s="254"/>
+      <c r="A141" s="250"/>
       <c r="B141" s="137" t="s">
         <v>253</v>
       </c>
@@ -13774,7 +13772,7 @@
       <c r="BD141" s="89"/>
     </row>
     <row r="142" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A142" s="254"/>
+      <c r="A142" s="250"/>
       <c r="B142" s="136" t="s">
         <v>254</v>
       </c>
@@ -13836,7 +13834,7 @@
       <c r="BD142" s="89"/>
     </row>
     <row r="143" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A143" s="254"/>
+      <c r="A143" s="250"/>
       <c r="B143" s="137" t="s">
         <v>255</v>
       </c>
@@ -13904,7 +13902,7 @@
       <c r="BD143" s="89"/>
     </row>
     <row r="144" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A144" s="254"/>
+      <c r="A144" s="250"/>
       <c r="B144" s="136" t="s">
         <v>256</v>
       </c>
@@ -13966,7 +13964,7 @@
       <c r="BD144" s="89"/>
     </row>
     <row r="145" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A145" s="254"/>
+      <c r="A145" s="250"/>
       <c r="B145" s="137" t="s">
         <v>257</v>
       </c>
@@ -14034,7 +14032,7 @@
       <c r="BD145" s="89"/>
     </row>
     <row r="146" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A146" s="254"/>
+      <c r="A146" s="250"/>
       <c r="B146" s="136" t="s">
         <v>258</v>
       </c>
@@ -14096,7 +14094,7 @@
       <c r="BD146" s="89"/>
     </row>
     <row r="147" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A147" s="254"/>
+      <c r="A147" s="250"/>
       <c r="B147" s="137" t="s">
         <v>259</v>
       </c>
@@ -14164,7 +14162,7 @@
       <c r="BD147" s="89"/>
     </row>
     <row r="148" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A148" s="254"/>
+      <c r="A148" s="250"/>
       <c r="B148" s="136" t="s">
         <v>260</v>
       </c>
@@ -14226,7 +14224,7 @@
       <c r="BD148" s="89"/>
     </row>
     <row r="149" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A149" s="254"/>
+      <c r="A149" s="250"/>
       <c r="B149" s="137" t="s">
         <v>261</v>
       </c>
@@ -14294,7 +14292,7 @@
       <c r="BD149" s="89"/>
     </row>
     <row r="150" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A150" s="254"/>
+      <c r="A150" s="250"/>
       <c r="B150" s="137" t="s">
         <v>262</v>
       </c>
@@ -14362,7 +14360,7 @@
       <c r="BD150" s="89"/>
     </row>
     <row r="151" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A151" s="254"/>
+      <c r="A151" s="250"/>
       <c r="B151" s="137" t="s">
         <v>263</v>
       </c>
@@ -14430,7 +14428,7 @@
       <c r="BD151" s="89"/>
     </row>
     <row r="152" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A152" s="254"/>
+      <c r="A152" s="250"/>
       <c r="B152" s="137" t="s">
         <v>264</v>
       </c>
@@ -14498,7 +14496,7 @@
       <c r="BD152" s="89"/>
     </row>
     <row r="153" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A153" s="254"/>
+      <c r="A153" s="250"/>
       <c r="B153" s="136" t="s">
         <v>265</v>
       </c>
@@ -14560,7 +14558,7 @@
       <c r="BD153" s="89"/>
     </row>
     <row r="154" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A154" s="254"/>
+      <c r="A154" s="250"/>
       <c r="B154" s="137" t="s">
         <v>266</v>
       </c>
@@ -14628,7 +14626,7 @@
       <c r="BD154" s="89"/>
     </row>
     <row r="155" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A155" s="254"/>
+      <c r="A155" s="250"/>
       <c r="B155" s="137" t="s">
         <v>267</v>
       </c>
@@ -14696,7 +14694,7 @@
       <c r="BD155" s="89"/>
     </row>
     <row r="156" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A156" s="254"/>
+      <c r="A156" s="250"/>
       <c r="B156" s="136" t="s">
         <v>268</v>
       </c>
@@ -14758,7 +14756,7 @@
       <c r="BD156" s="89"/>
     </row>
     <row r="157" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A157" s="254"/>
+      <c r="A157" s="250"/>
       <c r="B157" s="137" t="s">
         <v>269</v>
       </c>
@@ -14826,7 +14824,7 @@
       <c r="BD157" s="89"/>
     </row>
     <row r="158" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A158" s="254"/>
+      <c r="A158" s="250"/>
       <c r="B158" s="137" t="s">
         <v>270</v>
       </c>
@@ -14894,7 +14892,7 @@
       <c r="BD158" s="89"/>
     </row>
     <row r="159" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A159" s="254"/>
+      <c r="A159" s="250"/>
       <c r="B159" s="137" t="s">
         <v>271</v>
       </c>
@@ -14962,7 +14960,7 @@
       <c r="BD159" s="89"/>
     </row>
     <row r="160" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A160" s="254"/>
+      <c r="A160" s="250"/>
       <c r="B160" s="137" t="s">
         <v>272</v>
       </c>
@@ -15030,7 +15028,7 @@
       <c r="BD160" s="89"/>
     </row>
     <row r="161" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A161" s="254"/>
+      <c r="A161" s="250"/>
       <c r="B161" s="136" t="s">
         <v>273</v>
       </c>
@@ -15092,7 +15090,7 @@
       <c r="BD161" s="89"/>
     </row>
     <row r="162" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A162" s="254"/>
+      <c r="A162" s="250"/>
       <c r="B162" s="137" t="s">
         <v>274</v>
       </c>
@@ -15160,7 +15158,7 @@
       <c r="BD162" s="89"/>
     </row>
     <row r="163" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A163" s="254"/>
+      <c r="A163" s="250"/>
       <c r="B163" s="137" t="s">
         <v>275</v>
       </c>
@@ -15228,7 +15226,7 @@
       <c r="BD163" s="89"/>
     </row>
     <row r="164" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A164" s="254"/>
+      <c r="A164" s="250"/>
       <c r="B164" s="136" t="s">
         <v>276</v>
       </c>
@@ -15290,7 +15288,7 @@
       <c r="BD164" s="89"/>
     </row>
     <row r="165" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A165" s="254"/>
+      <c r="A165" s="250"/>
       <c r="B165" s="137" t="s">
         <v>277</v>
       </c>
@@ -15358,7 +15356,7 @@
       <c r="BD165" s="89"/>
     </row>
     <row r="166" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A166" s="254"/>
+      <c r="A166" s="250"/>
       <c r="B166" s="137" t="s">
         <v>278</v>
       </c>
@@ -15426,7 +15424,7 @@
       <c r="BD166" s="89"/>
     </row>
     <row r="167" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A167" s="254"/>
+      <c r="A167" s="250"/>
       <c r="B167" s="136" t="s">
         <v>279</v>
       </c>
@@ -15488,7 +15486,7 @@
       <c r="BD167" s="89"/>
     </row>
     <row r="168" spans="1:56" s="80" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A168" s="255"/>
+      <c r="A168" s="256"/>
       <c r="B168" s="138" t="s">
         <v>280</v>
       </c>
@@ -15628,74 +15626,74 @@
         <f>SUM(K170:BD170)</f>
         <v>3500</v>
       </c>
-      <c r="E170" s="238" t="s">
+      <c r="E170" s="271" t="s">
         <v>324</v>
       </c>
-      <c r="F170" s="238"/>
-      <c r="G170" s="238"/>
-      <c r="H170" s="233"/>
-      <c r="I170" s="231"/>
-      <c r="J170" s="231"/>
-      <c r="K170" s="231">
+      <c r="F170" s="271"/>
+      <c r="G170" s="271"/>
+      <c r="H170" s="263"/>
+      <c r="I170" s="261"/>
+      <c r="J170" s="261"/>
+      <c r="K170" s="261">
         <v>500</v>
       </c>
-      <c r="L170" s="231"/>
-      <c r="M170" s="231"/>
-      <c r="N170" s="232"/>
-      <c r="O170" s="233"/>
-      <c r="P170" s="231"/>
-      <c r="Q170" s="231"/>
-      <c r="R170" s="231">
+      <c r="L170" s="261"/>
+      <c r="M170" s="261"/>
+      <c r="N170" s="262"/>
+      <c r="O170" s="263"/>
+      <c r="P170" s="261"/>
+      <c r="Q170" s="261"/>
+      <c r="R170" s="261">
         <v>500</v>
       </c>
-      <c r="S170" s="231"/>
-      <c r="T170" s="231"/>
-      <c r="U170" s="232"/>
-      <c r="V170" s="233"/>
-      <c r="W170" s="231"/>
-      <c r="X170" s="231"/>
-      <c r="Y170" s="231">
+      <c r="S170" s="261"/>
+      <c r="T170" s="261"/>
+      <c r="U170" s="262"/>
+      <c r="V170" s="263"/>
+      <c r="W170" s="261"/>
+      <c r="X170" s="261"/>
+      <c r="Y170" s="261">
         <v>500</v>
       </c>
-      <c r="Z170" s="231"/>
-      <c r="AA170" s="231"/>
-      <c r="AB170" s="232"/>
-      <c r="AC170" s="233"/>
-      <c r="AD170" s="231"/>
-      <c r="AE170" s="231"/>
-      <c r="AF170" s="231">
+      <c r="Z170" s="261"/>
+      <c r="AA170" s="261"/>
+      <c r="AB170" s="262"/>
+      <c r="AC170" s="263"/>
+      <c r="AD170" s="261"/>
+      <c r="AE170" s="261"/>
+      <c r="AF170" s="261">
         <v>500</v>
       </c>
-      <c r="AG170" s="231"/>
-      <c r="AH170" s="231"/>
-      <c r="AI170" s="232"/>
-      <c r="AJ170" s="233"/>
-      <c r="AK170" s="231"/>
-      <c r="AL170" s="231"/>
-      <c r="AM170" s="231">
+      <c r="AG170" s="261"/>
+      <c r="AH170" s="261"/>
+      <c r="AI170" s="262"/>
+      <c r="AJ170" s="263"/>
+      <c r="AK170" s="261"/>
+      <c r="AL170" s="261"/>
+      <c r="AM170" s="261">
         <v>500</v>
       </c>
-      <c r="AN170" s="231"/>
-      <c r="AO170" s="231"/>
-      <c r="AP170" s="232"/>
-      <c r="AQ170" s="233"/>
-      <c r="AR170" s="231"/>
-      <c r="AS170" s="231"/>
-      <c r="AT170" s="231">
+      <c r="AN170" s="261"/>
+      <c r="AO170" s="261"/>
+      <c r="AP170" s="262"/>
+      <c r="AQ170" s="263"/>
+      <c r="AR170" s="261"/>
+      <c r="AS170" s="261"/>
+      <c r="AT170" s="261">
         <v>500</v>
       </c>
-      <c r="AU170" s="231"/>
-      <c r="AV170" s="231"/>
-      <c r="AW170" s="232"/>
-      <c r="AX170" s="233"/>
-      <c r="AY170" s="231"/>
-      <c r="AZ170" s="231"/>
-      <c r="BA170" s="231">
+      <c r="AU170" s="261"/>
+      <c r="AV170" s="261"/>
+      <c r="AW170" s="262"/>
+      <c r="AX170" s="263"/>
+      <c r="AY170" s="261"/>
+      <c r="AZ170" s="261"/>
+      <c r="BA170" s="261">
         <v>500</v>
       </c>
-      <c r="BB170" s="231"/>
-      <c r="BC170" s="231"/>
-      <c r="BD170" s="232"/>
+      <c r="BB170" s="261"/>
+      <c r="BC170" s="261"/>
+      <c r="BD170" s="262"/>
     </row>
     <row r="171" spans="1:56" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A171" s="150"/>
@@ -15707,74 +15705,74 @@
         <f>SUM(K171:BD171)</f>
         <v>4410</v>
       </c>
-      <c r="E171" s="238" t="s">
+      <c r="E171" s="271" t="s">
         <v>323</v>
       </c>
-      <c r="F171" s="238"/>
-      <c r="G171" s="238"/>
-      <c r="H171" s="233"/>
-      <c r="I171" s="231"/>
-      <c r="J171" s="231"/>
-      <c r="K171" s="231">
+      <c r="F171" s="271"/>
+      <c r="G171" s="271"/>
+      <c r="H171" s="263"/>
+      <c r="I171" s="261"/>
+      <c r="J171" s="261"/>
+      <c r="K171" s="261">
         <v>630</v>
       </c>
-      <c r="L171" s="231"/>
-      <c r="M171" s="231"/>
-      <c r="N171" s="232"/>
-      <c r="O171" s="233"/>
-      <c r="P171" s="231"/>
-      <c r="Q171" s="231"/>
-      <c r="R171" s="231">
+      <c r="L171" s="261"/>
+      <c r="M171" s="261"/>
+      <c r="N171" s="262"/>
+      <c r="O171" s="263"/>
+      <c r="P171" s="261"/>
+      <c r="Q171" s="261"/>
+      <c r="R171" s="261">
         <v>630</v>
       </c>
-      <c r="S171" s="231"/>
-      <c r="T171" s="231"/>
-      <c r="U171" s="232"/>
-      <c r="V171" s="233"/>
-      <c r="W171" s="231"/>
-      <c r="X171" s="231"/>
-      <c r="Y171" s="231">
+      <c r="S171" s="261"/>
+      <c r="T171" s="261"/>
+      <c r="U171" s="262"/>
+      <c r="V171" s="263"/>
+      <c r="W171" s="261"/>
+      <c r="X171" s="261"/>
+      <c r="Y171" s="261">
         <v>630</v>
       </c>
-      <c r="Z171" s="231"/>
-      <c r="AA171" s="231"/>
-      <c r="AB171" s="232"/>
-      <c r="AC171" s="233"/>
-      <c r="AD171" s="231"/>
-      <c r="AE171" s="231"/>
-      <c r="AF171" s="231">
+      <c r="Z171" s="261"/>
+      <c r="AA171" s="261"/>
+      <c r="AB171" s="262"/>
+      <c r="AC171" s="263"/>
+      <c r="AD171" s="261"/>
+      <c r="AE171" s="261"/>
+      <c r="AF171" s="261">
         <v>630</v>
       </c>
-      <c r="AG171" s="231"/>
-      <c r="AH171" s="231"/>
-      <c r="AI171" s="232"/>
-      <c r="AJ171" s="233"/>
-      <c r="AK171" s="231"/>
-      <c r="AL171" s="231"/>
-      <c r="AM171" s="231">
+      <c r="AG171" s="261"/>
+      <c r="AH171" s="261"/>
+      <c r="AI171" s="262"/>
+      <c r="AJ171" s="263"/>
+      <c r="AK171" s="261"/>
+      <c r="AL171" s="261"/>
+      <c r="AM171" s="261">
         <v>630</v>
       </c>
-      <c r="AN171" s="231"/>
-      <c r="AO171" s="231"/>
-      <c r="AP171" s="232"/>
-      <c r="AQ171" s="233"/>
-      <c r="AR171" s="231"/>
-      <c r="AS171" s="231"/>
-      <c r="AT171" s="231">
+      <c r="AN171" s="261"/>
+      <c r="AO171" s="261"/>
+      <c r="AP171" s="262"/>
+      <c r="AQ171" s="263"/>
+      <c r="AR171" s="261"/>
+      <c r="AS171" s="261"/>
+      <c r="AT171" s="261">
         <v>630</v>
       </c>
-      <c r="AU171" s="231"/>
-      <c r="AV171" s="231"/>
-      <c r="AW171" s="232"/>
-      <c r="AX171" s="233"/>
-      <c r="AY171" s="231"/>
-      <c r="AZ171" s="231"/>
-      <c r="BA171" s="231">
+      <c r="AU171" s="261"/>
+      <c r="AV171" s="261"/>
+      <c r="AW171" s="262"/>
+      <c r="AX171" s="263"/>
+      <c r="AY171" s="261"/>
+      <c r="AZ171" s="261"/>
+      <c r="BA171" s="261">
         <v>630</v>
       </c>
-      <c r="BB171" s="231"/>
-      <c r="BC171" s="231"/>
-      <c r="BD171" s="232"/>
+      <c r="BB171" s="261"/>
+      <c r="BC171" s="261"/>
+      <c r="BD171" s="262"/>
     </row>
     <row r="172" spans="1:56" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A172" s="152"/>
@@ -15786,74 +15784,74 @@
         <f>+D169+D171</f>
         <v>9910</v>
       </c>
-      <c r="E172" s="247" t="s">
+      <c r="E172" s="264" t="s">
         <v>307</v>
       </c>
-      <c r="F172" s="247"/>
-      <c r="G172" s="247"/>
-      <c r="H172" s="249"/>
-      <c r="I172" s="250"/>
-      <c r="J172" s="250"/>
-      <c r="K172" s="251">
+      <c r="F172" s="264"/>
+      <c r="G172" s="264"/>
+      <c r="H172" s="259"/>
+      <c r="I172" s="260"/>
+      <c r="J172" s="260"/>
+      <c r="K172" s="257">
         <v>44607</v>
       </c>
-      <c r="L172" s="251"/>
-      <c r="M172" s="251"/>
-      <c r="N172" s="252"/>
-      <c r="O172" s="249"/>
-      <c r="P172" s="250"/>
-      <c r="Q172" s="250"/>
-      <c r="R172" s="251">
+      <c r="L172" s="257"/>
+      <c r="M172" s="257"/>
+      <c r="N172" s="258"/>
+      <c r="O172" s="259"/>
+      <c r="P172" s="260"/>
+      <c r="Q172" s="260"/>
+      <c r="R172" s="257">
         <v>44607</v>
       </c>
-      <c r="S172" s="251"/>
-      <c r="T172" s="251"/>
-      <c r="U172" s="252"/>
-      <c r="V172" s="249"/>
-      <c r="W172" s="250"/>
-      <c r="X172" s="250"/>
-      <c r="Y172" s="251">
+      <c r="S172" s="257"/>
+      <c r="T172" s="257"/>
+      <c r="U172" s="258"/>
+      <c r="V172" s="259"/>
+      <c r="W172" s="260"/>
+      <c r="X172" s="260"/>
+      <c r="Y172" s="257">
         <v>44607</v>
       </c>
-      <c r="Z172" s="251"/>
-      <c r="AA172" s="251"/>
-      <c r="AB172" s="252"/>
-      <c r="AC172" s="249"/>
-      <c r="AD172" s="250"/>
-      <c r="AE172" s="250"/>
-      <c r="AF172" s="251">
+      <c r="Z172" s="257"/>
+      <c r="AA172" s="257"/>
+      <c r="AB172" s="258"/>
+      <c r="AC172" s="259"/>
+      <c r="AD172" s="260"/>
+      <c r="AE172" s="260"/>
+      <c r="AF172" s="257">
         <v>44607</v>
       </c>
-      <c r="AG172" s="251"/>
-      <c r="AH172" s="251"/>
-      <c r="AI172" s="252"/>
-      <c r="AJ172" s="249"/>
-      <c r="AK172" s="250"/>
-      <c r="AL172" s="250"/>
-      <c r="AM172" s="251">
+      <c r="AG172" s="257"/>
+      <c r="AH172" s="257"/>
+      <c r="AI172" s="258"/>
+      <c r="AJ172" s="259"/>
+      <c r="AK172" s="260"/>
+      <c r="AL172" s="260"/>
+      <c r="AM172" s="257">
         <v>44607</v>
       </c>
-      <c r="AN172" s="251"/>
-      <c r="AO172" s="251"/>
-      <c r="AP172" s="252"/>
-      <c r="AQ172" s="249"/>
-      <c r="AR172" s="250"/>
-      <c r="AS172" s="250"/>
-      <c r="AT172" s="251">
+      <c r="AN172" s="257"/>
+      <c r="AO172" s="257"/>
+      <c r="AP172" s="258"/>
+      <c r="AQ172" s="259"/>
+      <c r="AR172" s="260"/>
+      <c r="AS172" s="260"/>
+      <c r="AT172" s="257">
         <v>44607</v>
       </c>
-      <c r="AU172" s="251"/>
-      <c r="AV172" s="251"/>
-      <c r="AW172" s="252"/>
-      <c r="AX172" s="249"/>
-      <c r="AY172" s="250"/>
-      <c r="AZ172" s="250"/>
-      <c r="BA172" s="251">
+      <c r="AU172" s="257"/>
+      <c r="AV172" s="257"/>
+      <c r="AW172" s="258"/>
+      <c r="AX172" s="259"/>
+      <c r="AY172" s="260"/>
+      <c r="AZ172" s="260"/>
+      <c r="BA172" s="257">
         <v>44607</v>
       </c>
-      <c r="BB172" s="251"/>
-      <c r="BC172" s="251"/>
-      <c r="BD172" s="252"/>
+      <c r="BB172" s="257"/>
+      <c r="BC172" s="257"/>
+      <c r="BD172" s="258"/>
     </row>
     <row r="173" spans="1:56" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A173" s="163"/>
@@ -15978,59 +15976,22 @@
     </row>
   </sheetData>
   <mergeCells count="85">
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="D2:E2"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="AJ6:AP6"/>
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="C6:C7"/>
-    <mergeCell ref="A15:A30"/>
-    <mergeCell ref="A10:A12"/>
-    <mergeCell ref="O6:U6"/>
-    <mergeCell ref="V6:AB6"/>
-    <mergeCell ref="AC6:AI6"/>
-    <mergeCell ref="D6:D7"/>
-    <mergeCell ref="G6:G7"/>
-    <mergeCell ref="H6:N6"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="A104:A168"/>
-    <mergeCell ref="A80:A81"/>
-    <mergeCell ref="A83:A84"/>
-    <mergeCell ref="A87:A102"/>
-    <mergeCell ref="A32:A35"/>
-    <mergeCell ref="A37:A74"/>
-    <mergeCell ref="A77:A78"/>
-    <mergeCell ref="R172:U172"/>
-    <mergeCell ref="V172:X172"/>
-    <mergeCell ref="Y170:AB170"/>
-    <mergeCell ref="AC170:AE170"/>
-    <mergeCell ref="AF170:AI170"/>
-    <mergeCell ref="V170:X170"/>
-    <mergeCell ref="R170:U170"/>
-    <mergeCell ref="AQ172:AS172"/>
-    <mergeCell ref="AT172:AW172"/>
-    <mergeCell ref="AX172:AZ172"/>
-    <mergeCell ref="BA172:BD172"/>
-    <mergeCell ref="Y172:AB172"/>
-    <mergeCell ref="AC172:AE172"/>
-    <mergeCell ref="AF172:AI172"/>
-    <mergeCell ref="AJ172:AL172"/>
-    <mergeCell ref="AM172:AP172"/>
-    <mergeCell ref="E172:G172"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="I3:Q3"/>
-    <mergeCell ref="I4:Q4"/>
-    <mergeCell ref="H172:J172"/>
-    <mergeCell ref="K172:N172"/>
-    <mergeCell ref="O172:Q172"/>
-    <mergeCell ref="H170:J170"/>
-    <mergeCell ref="K170:N170"/>
-    <mergeCell ref="O170:Q170"/>
+    <mergeCell ref="AT171:AW171"/>
+    <mergeCell ref="AX171:AZ171"/>
+    <mergeCell ref="BA171:BD171"/>
+    <mergeCell ref="F2:BD2"/>
+    <mergeCell ref="F5:U5"/>
+    <mergeCell ref="R3:X3"/>
+    <mergeCell ref="R4:X4"/>
+    <mergeCell ref="E170:G170"/>
+    <mergeCell ref="AJ170:AL170"/>
+    <mergeCell ref="AM170:AP170"/>
+    <mergeCell ref="AT170:AW170"/>
+    <mergeCell ref="AX170:AZ170"/>
+    <mergeCell ref="BA170:BD170"/>
+    <mergeCell ref="AQ170:AS170"/>
+    <mergeCell ref="AQ6:AW6"/>
+    <mergeCell ref="AX6:BD6"/>
     <mergeCell ref="AL1:BD1"/>
     <mergeCell ref="O1:AG1"/>
     <mergeCell ref="AH1:AK1"/>
@@ -16047,22 +16008,59 @@
     <mergeCell ref="AJ171:AL171"/>
     <mergeCell ref="AM171:AP171"/>
     <mergeCell ref="AQ171:AS171"/>
-    <mergeCell ref="AT171:AW171"/>
-    <mergeCell ref="AX171:AZ171"/>
-    <mergeCell ref="BA171:BD171"/>
-    <mergeCell ref="F2:BD2"/>
-    <mergeCell ref="F5:U5"/>
-    <mergeCell ref="R3:X3"/>
-    <mergeCell ref="R4:X4"/>
-    <mergeCell ref="E170:G170"/>
-    <mergeCell ref="AJ170:AL170"/>
-    <mergeCell ref="AM170:AP170"/>
-    <mergeCell ref="AT170:AW170"/>
-    <mergeCell ref="AX170:AZ170"/>
-    <mergeCell ref="BA170:BD170"/>
-    <mergeCell ref="AQ170:AS170"/>
-    <mergeCell ref="AQ6:AW6"/>
-    <mergeCell ref="AX6:BD6"/>
+    <mergeCell ref="E172:G172"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="I3:Q3"/>
+    <mergeCell ref="I4:Q4"/>
+    <mergeCell ref="H172:J172"/>
+    <mergeCell ref="K172:N172"/>
+    <mergeCell ref="O172:Q172"/>
+    <mergeCell ref="H170:J170"/>
+    <mergeCell ref="K170:N170"/>
+    <mergeCell ref="O170:Q170"/>
+    <mergeCell ref="AQ172:AS172"/>
+    <mergeCell ref="AT172:AW172"/>
+    <mergeCell ref="AX172:AZ172"/>
+    <mergeCell ref="BA172:BD172"/>
+    <mergeCell ref="Y172:AB172"/>
+    <mergeCell ref="AC172:AE172"/>
+    <mergeCell ref="AF172:AI172"/>
+    <mergeCell ref="AJ172:AL172"/>
+    <mergeCell ref="AM172:AP172"/>
+    <mergeCell ref="R172:U172"/>
+    <mergeCell ref="V172:X172"/>
+    <mergeCell ref="Y170:AB170"/>
+    <mergeCell ref="AC170:AE170"/>
+    <mergeCell ref="AF170:AI170"/>
+    <mergeCell ref="V170:X170"/>
+    <mergeCell ref="R170:U170"/>
+    <mergeCell ref="A104:A168"/>
+    <mergeCell ref="A80:A81"/>
+    <mergeCell ref="A83:A84"/>
+    <mergeCell ref="A87:A102"/>
+    <mergeCell ref="A32:A35"/>
+    <mergeCell ref="A37:A74"/>
+    <mergeCell ref="A77:A78"/>
+    <mergeCell ref="AJ6:AP6"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="C6:C7"/>
+    <mergeCell ref="A15:A30"/>
+    <mergeCell ref="A10:A12"/>
+    <mergeCell ref="O6:U6"/>
+    <mergeCell ref="V6:AB6"/>
+    <mergeCell ref="AC6:AI6"/>
+    <mergeCell ref="D6:D7"/>
+    <mergeCell ref="G6:G7"/>
+    <mergeCell ref="H6:N6"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="D5:E5"/>
   </mergeCells>
   <phoneticPr fontId="5" type="noConversion"/>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
@@ -16084,8 +16082,8 @@
   </sheetPr>
   <dimension ref="B1:AG43"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A13" zoomScale="129" zoomScaleNormal="129" zoomScaleSheetLayoutView="129" workbookViewId="0">
-      <selection activeCell="J18" sqref="J18"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="129" zoomScaleNormal="129" zoomScaleSheetLayoutView="129" workbookViewId="0">
+      <selection activeCell="H19" sqref="H19:I19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
@@ -16107,15 +16105,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C1" s="277" t="s">
+      <c r="C1" s="300" t="s">
         <v>352</v>
       </c>
-      <c r="D1" s="277"/>
-      <c r="E1" s="277"/>
-      <c r="F1" s="277"/>
-      <c r="G1" s="277"/>
-      <c r="H1" s="277"/>
-      <c r="I1" s="277"/>
+      <c r="D1" s="300"/>
+      <c r="E1" s="300"/>
+      <c r="F1" s="300"/>
+      <c r="G1" s="300"/>
+      <c r="H1" s="300"/>
+      <c r="I1" s="300"/>
       <c r="J1" s="193"/>
       <c r="K1" s="193"/>
       <c r="L1" s="193"/>
@@ -16143,13 +16141,13 @@
     </row>
     <row r="2" spans="2:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B2" s="193"/>
-      <c r="C2" s="277"/>
-      <c r="D2" s="277"/>
-      <c r="E2" s="277"/>
-      <c r="F2" s="277"/>
-      <c r="G2" s="277"/>
-      <c r="H2" s="277"/>
-      <c r="I2" s="277"/>
+      <c r="C2" s="300"/>
+      <c r="D2" s="300"/>
+      <c r="E2" s="300"/>
+      <c r="F2" s="300"/>
+      <c r="G2" s="300"/>
+      <c r="H2" s="300"/>
+      <c r="I2" s="300"/>
       <c r="J2" s="193"/>
       <c r="K2" s="193"/>
       <c r="L2" s="193"/>
@@ -16176,11 +16174,11 @@
       <c r="AG2" s="182"/>
     </row>
     <row r="3" spans="2:33" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="216"/>
-      <c r="C3" s="216"/>
-      <c r="D3" s="216"/>
-      <c r="E3" s="216"/>
-      <c r="F3" s="216"/>
+      <c r="B3" s="215"/>
+      <c r="C3" s="215"/>
+      <c r="D3" s="215"/>
+      <c r="E3" s="215"/>
+      <c r="F3" s="215"/>
       <c r="G3" s="192"/>
       <c r="H3" s="192"/>
       <c r="I3" s="193"/>
@@ -16210,18 +16208,17 @@
       <c r="AG3" s="182"/>
     </row>
     <row r="4" spans="2:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="192"/>
-      <c r="C4" s="203" t="s">
-        <v>360</v>
-      </c>
-      <c r="D4" s="330" t="s">
-        <v>362</v>
-      </c>
-      <c r="E4" s="330"/>
-      <c r="F4" s="330"/>
-      <c r="G4" s="330"/>
-      <c r="H4" s="330"/>
-      <c r="I4" s="331"/>
+      <c r="C4" s="202" t="s">
+        <v>294</v>
+      </c>
+      <c r="D4" s="298" t="s">
+        <v>364</v>
+      </c>
+      <c r="E4" s="298"/>
+      <c r="F4" s="298"/>
+      <c r="G4" s="298"/>
+      <c r="H4" s="298"/>
+      <c r="I4" s="299"/>
       <c r="J4" s="193"/>
       <c r="K4" s="193"/>
       <c r="L4" s="193"/>
@@ -16248,17 +16245,17 @@
       <c r="AG4" s="182"/>
     </row>
     <row r="5" spans="2:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C5" s="203" t="s">
-        <v>361</v>
-      </c>
-      <c r="D5" s="332" t="s">
-        <v>363</v>
-      </c>
-      <c r="E5" s="332"/>
-      <c r="F5" s="332"/>
-      <c r="G5" s="332"/>
-      <c r="H5" s="332"/>
-      <c r="I5" s="333"/>
+      <c r="C5" s="202" t="s">
+        <v>341</v>
+      </c>
+      <c r="D5" s="298" t="s">
+        <v>344</v>
+      </c>
+      <c r="E5" s="298"/>
+      <c r="F5" s="298"/>
+      <c r="G5" s="298"/>
+      <c r="H5" s="298"/>
+      <c r="I5" s="299"/>
       <c r="J5" s="193"/>
       <c r="K5" s="193"/>
       <c r="L5" s="193"/>
@@ -16285,6 +16282,15 @@
       <c r="AG5" s="182"/>
     </row>
     <row r="6" spans="2:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C6" s="202" t="s">
+        <v>353</v>
+      </c>
+      <c r="D6" s="303"/>
+      <c r="E6" s="303"/>
+      <c r="F6" s="303"/>
+      <c r="G6" s="303"/>
+      <c r="H6" s="303"/>
+      <c r="I6" s="304"/>
       <c r="J6" s="193"/>
       <c r="K6" s="193"/>
       <c r="L6" s="193"/>
@@ -16311,17 +16317,18 @@
       <c r="AG6" s="182"/>
     </row>
     <row r="7" spans="2:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C7" s="203" t="s">
-        <v>294</v>
-      </c>
-      <c r="D7" s="330" t="s">
-        <v>364</v>
-      </c>
-      <c r="E7" s="330"/>
-      <c r="F7" s="330"/>
-      <c r="G7" s="330"/>
-      <c r="H7" s="330"/>
-      <c r="I7" s="331"/>
+      <c r="B7" s="192"/>
+      <c r="C7" s="202" t="s">
+        <v>359</v>
+      </c>
+      <c r="D7" s="305" t="s">
+        <v>351</v>
+      </c>
+      <c r="E7" s="305"/>
+      <c r="F7" s="305"/>
+      <c r="G7" s="305"/>
+      <c r="H7" s="305"/>
+      <c r="I7" s="306"/>
       <c r="J7" s="193"/>
       <c r="K7" s="193"/>
       <c r="L7" s="193"/>
@@ -16349,18 +16356,14 @@
     </row>
     <row r="8" spans="2:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B8" s="192"/>
-      <c r="C8" s="203" t="s">
-        <v>341</v>
-      </c>
-      <c r="D8" s="330" t="s">
-        <v>344</v>
-      </c>
-      <c r="E8" s="330"/>
-      <c r="F8" s="330"/>
-      <c r="G8" s="330"/>
-      <c r="H8" s="330"/>
-      <c r="I8" s="331"/>
-      <c r="J8" s="193"/>
+      <c r="C8" s="194"/>
+      <c r="D8" s="182"/>
+      <c r="E8" s="182"/>
+      <c r="F8" s="182"/>
+      <c r="G8" s="182"/>
+      <c r="H8" s="192"/>
+      <c r="I8" s="193"/>
+      <c r="J8" s="201"/>
       <c r="K8" s="193"/>
       <c r="L8" s="193"/>
       <c r="M8" s="193"/>
@@ -16387,16 +16390,16 @@
     </row>
     <row r="9" spans="2:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B9" s="192"/>
-      <c r="C9" s="203" t="s">
-        <v>353</v>
-      </c>
-      <c r="D9" s="275"/>
-      <c r="E9" s="275"/>
-      <c r="F9" s="275"/>
-      <c r="G9" s="275"/>
-      <c r="H9" s="275"/>
-      <c r="I9" s="276"/>
-      <c r="J9" s="202"/>
+      <c r="C9" s="200" t="s">
+        <v>365</v>
+      </c>
+      <c r="D9" s="298"/>
+      <c r="E9" s="298"/>
+      <c r="F9" s="298"/>
+      <c r="G9" s="298"/>
+      <c r="H9" s="298"/>
+      <c r="I9" s="299"/>
+      <c r="J9" s="193"/>
       <c r="K9" s="193"/>
       <c r="L9" s="193"/>
       <c r="M9" s="193"/>
@@ -16423,17 +16426,13 @@
     </row>
     <row r="10" spans="2:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B10" s="192"/>
-      <c r="C10" s="203" t="s">
-        <v>359</v>
-      </c>
-      <c r="D10" s="320" t="s">
-        <v>351</v>
-      </c>
-      <c r="E10" s="320"/>
-      <c r="F10" s="320"/>
-      <c r="G10" s="320"/>
-      <c r="H10" s="320"/>
-      <c r="I10" s="321"/>
+      <c r="C10" s="190"/>
+      <c r="D10" s="182"/>
+      <c r="E10" s="182"/>
+      <c r="F10" s="182"/>
+      <c r="G10" s="182"/>
+      <c r="H10" s="182"/>
+      <c r="I10" s="182"/>
       <c r="J10" s="193"/>
       <c r="K10" s="193"/>
       <c r="L10" s="193"/>
@@ -16459,15 +16458,17 @@
       <c r="AF10" s="182"/>
       <c r="AG10" s="182"/>
     </row>
-    <row r="11" spans="2:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="192"/>
-      <c r="C11" s="194"/>
-      <c r="D11" s="182"/>
-      <c r="E11" s="182"/>
-      <c r="F11" s="182"/>
-      <c r="G11" s="182"/>
-      <c r="H11" s="192"/>
-      <c r="I11" s="193"/>
+    <row r="11" spans="2:33" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C11" s="200" t="s">
+        <v>354</v>
+      </c>
+      <c r="D11" s="230"/>
+      <c r="F11" s="309" t="s">
+        <v>357</v>
+      </c>
+      <c r="G11" s="310"/>
+      <c r="H11" s="305"/>
+      <c r="I11" s="306"/>
       <c r="J11" s="193"/>
       <c r="K11" s="193"/>
       <c r="L11" s="193"/>
@@ -16493,16 +16494,17 @@
       <c r="AF11" s="182"/>
       <c r="AG11" s="182"/>
     </row>
-    <row r="12" spans="2:33" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:33" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C12" s="200" t="s">
-        <v>365</v>
-      </c>
-      <c r="D12" s="330"/>
-      <c r="E12" s="330"/>
-      <c r="F12" s="330"/>
-      <c r="G12" s="330"/>
-      <c r="H12" s="330"/>
-      <c r="I12" s="331"/>
+        <v>355</v>
+      </c>
+      <c r="D12" s="230"/>
+      <c r="F12" s="309" t="s">
+        <v>358</v>
+      </c>
+      <c r="G12" s="310"/>
+      <c r="H12" s="307"/>
+      <c r="I12" s="308"/>
       <c r="J12" s="193"/>
       <c r="K12" s="193"/>
       <c r="L12" s="193"/>
@@ -16528,16 +16530,14 @@
       <c r="AF12" s="182"/>
       <c r="AG12" s="182"/>
     </row>
-    <row r="13" spans="2:33" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C13" s="190"/>
-      <c r="D13" s="182"/>
-      <c r="E13" s="182"/>
-      <c r="F13" s="182"/>
-      <c r="G13" s="182"/>
-      <c r="H13" s="182"/>
-      <c r="I13" s="182"/>
-      <c r="J13" s="193"/>
-      <c r="K13" s="193"/>
+    <row r="13" spans="2:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C13" s="200" t="s">
+        <v>356</v>
+      </c>
+      <c r="D13" s="231"/>
+      <c r="E13" s="188"/>
+      <c r="F13" s="188"/>
+      <c r="I13" s="193"/>
       <c r="L13" s="193"/>
       <c r="M13" s="193"/>
       <c r="N13" s="193"/>
@@ -16562,16 +16562,11 @@
       <c r="AG13" s="182"/>
     </row>
     <row r="14" spans="2:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C14" s="200" t="s">
-        <v>354</v>
-      </c>
-      <c r="D14" s="324"/>
-      <c r="F14" s="282" t="s">
-        <v>357</v>
-      </c>
-      <c r="G14" s="283"/>
-      <c r="H14" s="320"/>
-      <c r="I14" s="321"/>
+      <c r="C14" s="339"/>
+      <c r="D14" s="340"/>
+      <c r="E14" s="188"/>
+      <c r="F14" s="188"/>
+      <c r="I14" s="193"/>
       <c r="L14" s="193"/>
       <c r="M14" s="193"/>
       <c r="N14" s="193"/>
@@ -16596,16 +16591,17 @@
       <c r="AG14" s="182"/>
     </row>
     <row r="15" spans="2:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C15" s="200" t="s">
-        <v>355</v>
-      </c>
-      <c r="D15" s="324"/>
-      <c r="F15" s="282" t="s">
-        <v>358</v>
-      </c>
-      <c r="G15" s="283"/>
-      <c r="H15" s="322"/>
-      <c r="I15" s="323"/>
+      <c r="C15" s="202" t="s">
+        <v>360</v>
+      </c>
+      <c r="D15" s="298" t="s">
+        <v>362</v>
+      </c>
+      <c r="E15" s="298"/>
+      <c r="F15" s="298"/>
+      <c r="G15" s="298"/>
+      <c r="H15" s="298"/>
+      <c r="I15" s="299"/>
       <c r="L15" s="193"/>
       <c r="M15" s="193"/>
       <c r="N15" s="193"/>
@@ -16626,13 +16622,17 @@
       <c r="AC15" s="193"/>
     </row>
     <row r="16" spans="2:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C16" s="201" t="s">
-        <v>356</v>
-      </c>
-      <c r="D16" s="329"/>
-      <c r="E16" s="188"/>
-      <c r="F16" s="188"/>
-      <c r="I16" s="193"/>
+      <c r="C16" s="202" t="s">
+        <v>361</v>
+      </c>
+      <c r="D16" s="301" t="s">
+        <v>363</v>
+      </c>
+      <c r="E16" s="301"/>
+      <c r="F16" s="301"/>
+      <c r="G16" s="301"/>
+      <c r="H16" s="301"/>
+      <c r="I16" s="302"/>
       <c r="J16" s="193"/>
       <c r="K16" s="193"/>
       <c r="L16" s="193"/>
@@ -16682,23 +16682,23 @@
       <c r="AC17" s="193"/>
     </row>
     <row r="18" spans="2:33" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C18" s="278" t="s">
+      <c r="C18" s="276" t="s">
         <v>305</v>
       </c>
-      <c r="D18" s="279"/>
-      <c r="E18" s="279"/>
-      <c r="F18" s="279"/>
-      <c r="G18" s="279"/>
-      <c r="H18" s="340"/>
-      <c r="I18" s="341"/>
-      <c r="K18" s="213"/>
-      <c r="L18" s="213"/>
-      <c r="M18" s="213"/>
-      <c r="N18" s="213"/>
-      <c r="O18" s="213"/>
-      <c r="P18" s="213"/>
-      <c r="Q18" s="213"/>
-      <c r="R18" s="213"/>
+      <c r="D18" s="277"/>
+      <c r="E18" s="277"/>
+      <c r="F18" s="277"/>
+      <c r="G18" s="277"/>
+      <c r="H18" s="278"/>
+      <c r="I18" s="279"/>
+      <c r="K18" s="212"/>
+      <c r="L18" s="212"/>
+      <c r="M18" s="212"/>
+      <c r="N18" s="212"/>
+      <c r="O18" s="212"/>
+      <c r="P18" s="212"/>
+      <c r="Q18" s="212"/>
+      <c r="R18" s="212"/>
       <c r="S18" s="187"/>
       <c r="T18" s="187"/>
       <c r="U18" s="187"/>
@@ -16719,16 +16719,16 @@
       <c r="E19" s="281"/>
       <c r="F19" s="281"/>
       <c r="G19" s="281"/>
-      <c r="H19" s="328"/>
-      <c r="I19" s="327"/>
-      <c r="K19" s="213"/>
-      <c r="L19" s="213"/>
-      <c r="M19" s="213"/>
-      <c r="N19" s="213"/>
-      <c r="O19" s="213"/>
-      <c r="P19" s="213"/>
-      <c r="Q19" s="213"/>
-      <c r="R19" s="213"/>
+      <c r="H19" s="341"/>
+      <c r="I19" s="342"/>
+      <c r="K19" s="212"/>
+      <c r="L19" s="212"/>
+      <c r="M19" s="212"/>
+      <c r="N19" s="212"/>
+      <c r="O19" s="212"/>
+      <c r="P19" s="212"/>
+      <c r="Q19" s="212"/>
+      <c r="R19" s="212"/>
       <c r="S19" s="187"/>
       <c r="T19" s="187"/>
       <c r="U19" s="187"/>
@@ -16742,26 +16742,26 @@
       <c r="AC19" s="186"/>
     </row>
     <row r="20" spans="2:33" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C20" s="325" t="s">
+      <c r="C20" s="282" t="s">
         <v>304</v>
       </c>
-      <c r="D20" s="326"/>
-      <c r="E20" s="326"/>
-      <c r="F20" s="326"/>
-      <c r="G20" s="326"/>
-      <c r="H20" s="336">
+      <c r="D20" s="283"/>
+      <c r="E20" s="283"/>
+      <c r="F20" s="283"/>
+      <c r="G20" s="283"/>
+      <c r="H20" s="284">
         <f>H18+H19</f>
         <v>0</v>
       </c>
-      <c r="I20" s="337"/>
-      <c r="K20" s="213"/>
-      <c r="L20" s="213"/>
-      <c r="M20" s="213"/>
-      <c r="N20" s="213"/>
-      <c r="O20" s="213"/>
-      <c r="P20" s="213"/>
-      <c r="Q20" s="213"/>
-      <c r="R20" s="213"/>
+      <c r="I20" s="285"/>
+      <c r="K20" s="212"/>
+      <c r="L20" s="212"/>
+      <c r="M20" s="212"/>
+      <c r="N20" s="212"/>
+      <c r="O20" s="212"/>
+      <c r="P20" s="212"/>
+      <c r="Q20" s="212"/>
+      <c r="R20" s="212"/>
       <c r="S20" s="187"/>
       <c r="T20" s="187"/>
       <c r="U20" s="187"/>
@@ -16776,14 +16776,14 @@
     </row>
     <row r="21" spans="2:33" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="G21" s="180"/>
-      <c r="K21" s="213"/>
-      <c r="L21" s="213"/>
-      <c r="M21" s="213"/>
-      <c r="N21" s="213"/>
-      <c r="O21" s="213"/>
-      <c r="P21" s="213"/>
-      <c r="Q21" s="213"/>
-      <c r="R21" s="213"/>
+      <c r="K21" s="212"/>
+      <c r="L21" s="212"/>
+      <c r="M21" s="212"/>
+      <c r="N21" s="212"/>
+      <c r="O21" s="212"/>
+      <c r="P21" s="212"/>
+      <c r="Q21" s="212"/>
+      <c r="R21" s="212"/>
       <c r="S21" s="187"/>
       <c r="T21" s="187"/>
       <c r="U21" s="187"/>
@@ -16797,21 +16797,21 @@
       <c r="AC21" s="186"/>
     </row>
     <row r="22" spans="2:33" s="182" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="303" t="s">
+      <c r="B22" s="311" t="s">
         <v>160</v>
       </c>
-      <c r="C22" s="304" t="s">
+      <c r="C22" s="296" t="s">
         <v>157</v>
       </c>
-      <c r="D22" s="305" t="s">
+      <c r="D22" s="288" t="s">
         <v>301</v>
       </c>
-      <c r="E22" s="306"/>
-      <c r="F22" s="306"/>
-      <c r="G22" s="306"/>
-      <c r="H22" s="306"/>
-      <c r="I22" s="307"/>
-      <c r="J22" s="308" t="s">
+      <c r="E22" s="289"/>
+      <c r="F22" s="289"/>
+      <c r="G22" s="289"/>
+      <c r="H22" s="289"/>
+      <c r="I22" s="290"/>
+      <c r="J22" s="318" t="s">
         <v>370</v>
       </c>
       <c r="K22" s="189"/>
@@ -16839,17 +16839,17 @@
       <c r="AG22" s="183"/>
     </row>
     <row r="23" spans="2:33" s="182" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="309"/>
-      <c r="C23" s="310"/>
-      <c r="D23" s="311" t="s">
+      <c r="B23" s="312"/>
+      <c r="C23" s="297"/>
+      <c r="D23" s="291" t="s">
         <v>340</v>
       </c>
-      <c r="E23" s="312"/>
-      <c r="F23" s="312"/>
-      <c r="G23" s="312"/>
-      <c r="H23" s="312"/>
-      <c r="I23" s="312"/>
-      <c r="J23" s="313"/>
+      <c r="E23" s="292"/>
+      <c r="F23" s="292"/>
+      <c r="G23" s="292"/>
+      <c r="H23" s="292"/>
+      <c r="I23" s="292"/>
+      <c r="J23" s="319"/>
       <c r="K23" s="190"/>
       <c r="L23" s="190"/>
       <c r="M23" s="190"/>
@@ -16868,78 +16868,78 @@
       <c r="Z23" s="190"/>
       <c r="AA23" s="190"/>
       <c r="AB23" s="190"/>
-      <c r="AC23" s="212"/>
+      <c r="AC23" s="211"/>
       <c r="AD23" s="183"/>
       <c r="AE23" s="183"/>
       <c r="AF23" s="183"/>
       <c r="AG23" s="183"/>
     </row>
     <row r="24" spans="2:33" s="182" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="309"/>
-      <c r="C24" s="310"/>
-      <c r="D24" s="314" t="s">
+      <c r="B24" s="312"/>
+      <c r="C24" s="297"/>
+      <c r="D24" s="286" t="s">
         <v>342</v>
       </c>
-      <c r="E24" s="314" t="s">
+      <c r="E24" s="286" t="s">
         <v>366</v>
       </c>
-      <c r="F24" s="315" t="s">
+      <c r="F24" s="293" t="s">
         <v>367</v>
       </c>
-      <c r="G24" s="315" t="s">
+      <c r="G24" s="293" t="s">
         <v>368</v>
       </c>
-      <c r="H24" s="315" t="s">
+      <c r="H24" s="293" t="s">
         <v>369</v>
       </c>
-      <c r="I24" s="314" t="s">
+      <c r="I24" s="286" t="s">
         <v>343</v>
       </c>
-      <c r="J24" s="313"/>
+      <c r="J24" s="319"/>
     </row>
     <row r="25" spans="2:33" s="182" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="309"/>
-      <c r="C25" s="310"/>
-      <c r="D25" s="314"/>
-      <c r="E25" s="314"/>
-      <c r="F25" s="316"/>
-      <c r="G25" s="316"/>
-      <c r="H25" s="316"/>
-      <c r="I25" s="314"/>
-      <c r="J25" s="313"/>
+      <c r="B25" s="312"/>
+      <c r="C25" s="297"/>
+      <c r="D25" s="286"/>
+      <c r="E25" s="286"/>
+      <c r="F25" s="294"/>
+      <c r="G25" s="294"/>
+      <c r="H25" s="294"/>
+      <c r="I25" s="286"/>
+      <c r="J25" s="319"/>
     </row>
     <row r="26" spans="2:33" s="182" customFormat="1" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="317"/>
-      <c r="C26" s="310"/>
-      <c r="D26" s="318"/>
-      <c r="E26" s="318"/>
-      <c r="F26" s="319"/>
-      <c r="G26" s="319"/>
-      <c r="H26" s="319"/>
-      <c r="I26" s="318"/>
-      <c r="J26" s="313"/>
+      <c r="B26" s="313"/>
+      <c r="C26" s="297"/>
+      <c r="D26" s="287"/>
+      <c r="E26" s="287"/>
+      <c r="F26" s="295"/>
+      <c r="G26" s="295"/>
+      <c r="H26" s="295"/>
+      <c r="I26" s="287"/>
+      <c r="J26" s="319"/>
     </row>
     <row r="27" spans="2:33" s="182" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="B27" s="217"/>
-      <c r="C27" s="218"/>
-      <c r="D27" s="219"/>
-      <c r="E27" s="220"/>
-      <c r="F27" s="338"/>
-      <c r="G27" s="221"/>
-      <c r="H27" s="221"/>
-      <c r="I27" s="222"/>
-      <c r="J27" s="223"/>
+      <c r="B27" s="216"/>
+      <c r="C27" s="217"/>
+      <c r="D27" s="218"/>
+      <c r="E27" s="219"/>
+      <c r="F27" s="234"/>
+      <c r="G27" s="220"/>
+      <c r="H27" s="220"/>
+      <c r="I27" s="221"/>
+      <c r="J27" s="222"/>
     </row>
     <row r="28" spans="2:33" s="182" customFormat="1" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="224"/>
-      <c r="C28" s="225"/>
-      <c r="D28" s="226"/>
-      <c r="E28" s="227"/>
-      <c r="F28" s="339"/>
-      <c r="G28" s="228"/>
-      <c r="H28" s="228"/>
-      <c r="I28" s="229"/>
-      <c r="J28" s="230"/>
+      <c r="B28" s="223"/>
+      <c r="C28" s="224"/>
+      <c r="D28" s="225"/>
+      <c r="E28" s="226"/>
+      <c r="F28" s="235"/>
+      <c r="G28" s="227"/>
+      <c r="H28" s="227"/>
+      <c r="I28" s="228"/>
+      <c r="J28" s="229"/>
     </row>
     <row r="29" spans="2:33" s="182" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B29" s="195"/>
@@ -16953,170 +16953,170 @@
     </row>
     <row r="30" spans="2:33" s="182" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B30" s="181"/>
-      <c r="C30" s="204" t="s">
+      <c r="C30" s="203" t="s">
         <v>346</v>
       </c>
-      <c r="D30" s="205"/>
-      <c r="E30" s="205"/>
-      <c r="F30" s="205"/>
-      <c r="G30" s="205"/>
-      <c r="H30" s="335"/>
-      <c r="I30" s="334"/>
-      <c r="J30" s="272"/>
-      <c r="K30" s="272"/>
-      <c r="L30" s="272"/>
-      <c r="M30" s="215"/>
-      <c r="N30" s="215"/>
-      <c r="O30" s="215"/>
+      <c r="D30" s="204"/>
+      <c r="E30" s="204"/>
+      <c r="F30" s="204"/>
+      <c r="G30" s="204"/>
+      <c r="H30" s="233"/>
+      <c r="I30" s="232"/>
+      <c r="J30" s="315"/>
+      <c r="K30" s="315"/>
+      <c r="L30" s="315"/>
+      <c r="M30" s="214"/>
+      <c r="N30" s="214"/>
+      <c r="O30" s="214"/>
       <c r="P30" s="191"/>
-      <c r="Q30" s="215"/>
-      <c r="R30" s="215"/>
-      <c r="S30" s="215"/>
-      <c r="T30" s="215"/>
-      <c r="U30" s="215"/>
-      <c r="V30" s="273"/>
-      <c r="W30" s="273"/>
-      <c r="X30" s="272"/>
-      <c r="Y30" s="272"/>
-      <c r="Z30" s="272"/>
-      <c r="AA30" s="272"/>
-      <c r="AB30" s="272"/>
-      <c r="AC30" s="213"/>
+      <c r="Q30" s="214"/>
+      <c r="R30" s="214"/>
+      <c r="S30" s="214"/>
+      <c r="T30" s="214"/>
+      <c r="U30" s="214"/>
+      <c r="V30" s="316"/>
+      <c r="W30" s="316"/>
+      <c r="X30" s="315"/>
+      <c r="Y30" s="315"/>
+      <c r="Z30" s="315"/>
+      <c r="AA30" s="315"/>
+      <c r="AB30" s="315"/>
+      <c r="AC30" s="212"/>
     </row>
     <row r="31" spans="2:33" s="182" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B31" s="181"/>
-      <c r="C31" s="206" t="s">
+      <c r="C31" s="205" t="s">
         <v>349</v>
       </c>
-      <c r="D31" s="207"/>
-      <c r="E31" s="207"/>
-      <c r="F31" s="207"/>
-      <c r="G31" s="207"/>
-      <c r="H31" s="335"/>
-      <c r="I31" s="334"/>
-      <c r="J31" s="213"/>
-      <c r="O31" s="215"/>
-      <c r="P31" s="215"/>
-      <c r="Q31" s="215"/>
-      <c r="R31" s="215"/>
-      <c r="S31" s="215"/>
-      <c r="T31" s="215"/>
-      <c r="U31" s="215"/>
-      <c r="V31" s="214"/>
-      <c r="W31" s="214"/>
-      <c r="X31" s="213"/>
-      <c r="Y31" s="213"/>
-      <c r="Z31" s="213"/>
-      <c r="AA31" s="213"/>
-      <c r="AB31" s="213"/>
-      <c r="AC31" s="213"/>
+      <c r="D31" s="206"/>
+      <c r="E31" s="206"/>
+      <c r="F31" s="206"/>
+      <c r="G31" s="206"/>
+      <c r="H31" s="233"/>
+      <c r="I31" s="232"/>
+      <c r="J31" s="212"/>
+      <c r="O31" s="214"/>
+      <c r="P31" s="214"/>
+      <c r="Q31" s="214"/>
+      <c r="R31" s="214"/>
+      <c r="S31" s="214"/>
+      <c r="T31" s="214"/>
+      <c r="U31" s="214"/>
+      <c r="V31" s="213"/>
+      <c r="W31" s="213"/>
+      <c r="X31" s="212"/>
+      <c r="Y31" s="212"/>
+      <c r="Z31" s="212"/>
+      <c r="AA31" s="212"/>
+      <c r="AB31" s="212"/>
+      <c r="AC31" s="212"/>
     </row>
     <row r="32" spans="2:33" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B32" s="181"/>
-      <c r="C32" s="208" t="s">
+      <c r="C32" s="207" t="s">
         <v>345</v>
       </c>
-      <c r="D32" s="209"/>
-      <c r="E32" s="209"/>
-      <c r="F32" s="209"/>
-      <c r="G32" s="209"/>
-      <c r="H32" s="335"/>
-      <c r="I32" s="334"/>
-      <c r="J32" s="272"/>
-      <c r="K32" s="272"/>
-      <c r="L32" s="272"/>
-      <c r="M32" s="215"/>
-      <c r="N32" s="215"/>
-      <c r="O32" s="215"/>
-      <c r="P32" s="215"/>
-      <c r="Q32" s="215"/>
-      <c r="R32" s="215"/>
-      <c r="S32" s="215"/>
-      <c r="T32" s="215"/>
-      <c r="U32" s="215"/>
-      <c r="V32" s="215"/>
-      <c r="W32" s="274"/>
-      <c r="X32" s="274"/>
-      <c r="Y32" s="274"/>
-      <c r="Z32" s="215"/>
-      <c r="AA32" s="215"/>
-      <c r="AB32" s="215"/>
-      <c r="AC32" s="215"/>
+      <c r="D32" s="208"/>
+      <c r="E32" s="208"/>
+      <c r="F32" s="208"/>
+      <c r="G32" s="208"/>
+      <c r="H32" s="233"/>
+      <c r="I32" s="232"/>
+      <c r="J32" s="315"/>
+      <c r="K32" s="315"/>
+      <c r="L32" s="315"/>
+      <c r="M32" s="214"/>
+      <c r="N32" s="214"/>
+      <c r="O32" s="214"/>
+      <c r="P32" s="214"/>
+      <c r="Q32" s="214"/>
+      <c r="R32" s="214"/>
+      <c r="S32" s="214"/>
+      <c r="T32" s="214"/>
+      <c r="U32" s="214"/>
+      <c r="V32" s="214"/>
+      <c r="W32" s="317"/>
+      <c r="X32" s="317"/>
+      <c r="Y32" s="317"/>
+      <c r="Z32" s="214"/>
+      <c r="AA32" s="214"/>
+      <c r="AB32" s="214"/>
+      <c r="AC32" s="214"/>
     </row>
     <row r="33" spans="2:29" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B33" s="181"/>
-      <c r="C33" s="208" t="s">
+      <c r="C33" s="207" t="s">
         <v>347</v>
       </c>
-      <c r="D33" s="209"/>
-      <c r="E33" s="209"/>
-      <c r="F33" s="209"/>
-      <c r="G33" s="209"/>
-      <c r="H33" s="335"/>
-      <c r="I33" s="334"/>
-      <c r="J33" s="215"/>
-      <c r="K33" s="215"/>
-      <c r="L33" s="215"/>
-      <c r="M33" s="215"/>
-      <c r="N33" s="215"/>
-      <c r="O33" s="215"/>
-      <c r="P33" s="215"/>
-      <c r="Q33" s="215"/>
-      <c r="R33" s="215"/>
-      <c r="S33" s="215"/>
-      <c r="T33" s="215"/>
-      <c r="U33" s="215"/>
-      <c r="V33" s="215"/>
-      <c r="W33" s="271"/>
-      <c r="X33" s="271"/>
-      <c r="Y33" s="271"/>
-      <c r="Z33" s="271"/>
-      <c r="AA33" s="271"/>
-      <c r="AB33" s="215"/>
-      <c r="AC33" s="215"/>
+      <c r="D33" s="208"/>
+      <c r="E33" s="208"/>
+      <c r="F33" s="208"/>
+      <c r="G33" s="208"/>
+      <c r="H33" s="233"/>
+      <c r="I33" s="232"/>
+      <c r="J33" s="214"/>
+      <c r="K33" s="214"/>
+      <c r="L33" s="214"/>
+      <c r="M33" s="214"/>
+      <c r="N33" s="214"/>
+      <c r="O33" s="214"/>
+      <c r="P33" s="214"/>
+      <c r="Q33" s="214"/>
+      <c r="R33" s="214"/>
+      <c r="S33" s="214"/>
+      <c r="T33" s="214"/>
+      <c r="U33" s="214"/>
+      <c r="V33" s="214"/>
+      <c r="W33" s="314"/>
+      <c r="X33" s="314"/>
+      <c r="Y33" s="314"/>
+      <c r="Z33" s="314"/>
+      <c r="AA33" s="314"/>
+      <c r="AB33" s="214"/>
+      <c r="AC33" s="214"/>
     </row>
     <row r="34" spans="2:29" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B34" s="181"/>
-      <c r="C34" s="206" t="s">
+      <c r="C34" s="205" t="s">
         <v>348</v>
       </c>
-      <c r="D34" s="207"/>
-      <c r="E34" s="207"/>
-      <c r="F34" s="207"/>
-      <c r="G34" s="207"/>
-      <c r="H34" s="335"/>
-      <c r="I34" s="334"/>
-      <c r="J34" s="215"/>
-      <c r="K34" s="215"/>
-      <c r="L34" s="215"/>
-      <c r="M34" s="215"/>
-      <c r="N34" s="215"/>
-      <c r="O34" s="215"/>
-      <c r="P34" s="215"/>
-      <c r="Q34" s="215"/>
-      <c r="R34" s="215"/>
-      <c r="S34" s="215"/>
-      <c r="T34" s="215"/>
-      <c r="U34" s="215"/>
-      <c r="V34" s="215"/>
-      <c r="W34" s="215"/>
-      <c r="X34" s="215"/>
-      <c r="Y34" s="215"/>
-      <c r="Z34" s="215"/>
-      <c r="AA34" s="215"/>
-      <c r="AB34" s="215"/>
-      <c r="AC34" s="215"/>
+      <c r="D34" s="206"/>
+      <c r="E34" s="206"/>
+      <c r="F34" s="206"/>
+      <c r="G34" s="206"/>
+      <c r="H34" s="233"/>
+      <c r="I34" s="232"/>
+      <c r="J34" s="214"/>
+      <c r="K34" s="214"/>
+      <c r="L34" s="214"/>
+      <c r="M34" s="214"/>
+      <c r="N34" s="214"/>
+      <c r="O34" s="214"/>
+      <c r="P34" s="214"/>
+      <c r="Q34" s="214"/>
+      <c r="R34" s="214"/>
+      <c r="S34" s="214"/>
+      <c r="T34" s="214"/>
+      <c r="U34" s="214"/>
+      <c r="V34" s="214"/>
+      <c r="W34" s="214"/>
+      <c r="X34" s="214"/>
+      <c r="Y34" s="214"/>
+      <c r="Z34" s="214"/>
+      <c r="AA34" s="214"/>
+      <c r="AB34" s="214"/>
+      <c r="AC34" s="214"/>
     </row>
     <row r="35" spans="2:29" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C35" s="210" t="s">
+      <c r="C35" s="209" t="s">
         <v>350</v>
       </c>
-      <c r="D35" s="211"/>
-      <c r="E35" s="211"/>
-      <c r="F35" s="211"/>
-      <c r="G35" s="211"/>
-      <c r="H35" s="335"/>
-      <c r="I35" s="334"/>
+      <c r="D35" s="210"/>
+      <c r="E35" s="210"/>
+      <c r="F35" s="210"/>
+      <c r="G35" s="210"/>
+      <c r="H35" s="233"/>
+      <c r="I35" s="232"/>
       <c r="J35" s="184"/>
       <c r="W35" s="185"/>
     </row>
@@ -17125,31 +17125,6 @@
     </row>
   </sheetData>
   <mergeCells count="35">
-    <mergeCell ref="C18:G18"/>
-    <mergeCell ref="H18:I18"/>
-    <mergeCell ref="C19:G19"/>
-    <mergeCell ref="C20:G20"/>
-    <mergeCell ref="H19:I19"/>
-    <mergeCell ref="H20:I20"/>
-    <mergeCell ref="E24:E26"/>
-    <mergeCell ref="D22:I22"/>
-    <mergeCell ref="D23:I23"/>
-    <mergeCell ref="F24:F26"/>
-    <mergeCell ref="G24:G26"/>
-    <mergeCell ref="H24:H26"/>
-    <mergeCell ref="C22:C26"/>
-    <mergeCell ref="D12:I12"/>
-    <mergeCell ref="C1:I2"/>
-    <mergeCell ref="D8:I8"/>
-    <mergeCell ref="D4:I4"/>
-    <mergeCell ref="D5:I5"/>
-    <mergeCell ref="D7:I7"/>
-    <mergeCell ref="D9:I9"/>
-    <mergeCell ref="D10:I10"/>
-    <mergeCell ref="H14:I14"/>
-    <mergeCell ref="H15:I15"/>
-    <mergeCell ref="F14:G14"/>
-    <mergeCell ref="F15:G15"/>
     <mergeCell ref="B22:B26"/>
     <mergeCell ref="W33:AA33"/>
     <mergeCell ref="D24:D26"/>
@@ -17160,6 +17135,31 @@
     <mergeCell ref="W32:Y32"/>
     <mergeCell ref="J30:L30"/>
     <mergeCell ref="J22:J26"/>
+    <mergeCell ref="C22:C26"/>
+    <mergeCell ref="D9:I9"/>
+    <mergeCell ref="C1:I2"/>
+    <mergeCell ref="D5:I5"/>
+    <mergeCell ref="D15:I15"/>
+    <mergeCell ref="D16:I16"/>
+    <mergeCell ref="D4:I4"/>
+    <mergeCell ref="D6:I6"/>
+    <mergeCell ref="D7:I7"/>
+    <mergeCell ref="H11:I11"/>
+    <mergeCell ref="H12:I12"/>
+    <mergeCell ref="F11:G11"/>
+    <mergeCell ref="F12:G12"/>
+    <mergeCell ref="E24:E26"/>
+    <mergeCell ref="D22:I22"/>
+    <mergeCell ref="D23:I23"/>
+    <mergeCell ref="F24:F26"/>
+    <mergeCell ref="G24:G26"/>
+    <mergeCell ref="H24:H26"/>
+    <mergeCell ref="C18:G18"/>
+    <mergeCell ref="H18:I18"/>
+    <mergeCell ref="C19:G19"/>
+    <mergeCell ref="C20:G20"/>
+    <mergeCell ref="H19:I19"/>
+    <mergeCell ref="H20:I20"/>
   </mergeCells>
   <phoneticPr fontId="5" type="noConversion"/>
   <conditionalFormatting sqref="P30">
@@ -17203,72 +17203,72 @@
   <sheetData>
     <row r="1" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="285" t="s">
+      <c r="B2" s="321" t="s">
         <v>62</v>
       </c>
-      <c r="C2" s="286"/>
-      <c r="D2" s="286"/>
-      <c r="E2" s="286"/>
-      <c r="F2" s="286"/>
-      <c r="G2" s="286"/>
-      <c r="H2" s="286"/>
-      <c r="I2" s="286"/>
-      <c r="J2" s="286"/>
-      <c r="K2" s="286"/>
-      <c r="L2" s="286"/>
-      <c r="M2" s="287"/>
+      <c r="C2" s="322"/>
+      <c r="D2" s="322"/>
+      <c r="E2" s="322"/>
+      <c r="F2" s="322"/>
+      <c r="G2" s="322"/>
+      <c r="H2" s="322"/>
+      <c r="I2" s="322"/>
+      <c r="J2" s="322"/>
+      <c r="K2" s="322"/>
+      <c r="L2" s="322"/>
+      <c r="M2" s="323"/>
     </row>
     <row r="3" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B3" s="288" t="s">
+      <c r="B3" s="324" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="290" t="s">
+      <c r="C3" s="326" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="290" t="s">
+      <c r="D3" s="326" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="292" t="s">
+      <c r="E3" s="328" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="294" t="s">
+      <c r="F3" s="330" t="s">
         <v>85</v>
       </c>
-      <c r="G3" s="295"/>
-      <c r="H3" s="295"/>
-      <c r="I3" s="295"/>
-      <c r="J3" s="295"/>
-      <c r="K3" s="295"/>
-      <c r="L3" s="295"/>
-      <c r="M3" s="296"/>
+      <c r="G3" s="331"/>
+      <c r="H3" s="331"/>
+      <c r="I3" s="331"/>
+      <c r="J3" s="331"/>
+      <c r="K3" s="331"/>
+      <c r="L3" s="331"/>
+      <c r="M3" s="332"/>
     </row>
     <row r="4" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="289"/>
-      <c r="C4" s="291"/>
-      <c r="D4" s="291"/>
-      <c r="E4" s="293"/>
-      <c r="F4" s="297"/>
-      <c r="G4" s="298"/>
-      <c r="H4" s="298"/>
-      <c r="I4" s="298"/>
-      <c r="J4" s="298"/>
-      <c r="K4" s="298"/>
-      <c r="L4" s="298"/>
-      <c r="M4" s="299"/>
+      <c r="B4" s="325"/>
+      <c r="C4" s="327"/>
+      <c r="D4" s="327"/>
+      <c r="E4" s="329"/>
+      <c r="F4" s="333"/>
+      <c r="G4" s="334"/>
+      <c r="H4" s="334"/>
+      <c r="I4" s="334"/>
+      <c r="J4" s="334"/>
+      <c r="K4" s="334"/>
+      <c r="L4" s="334"/>
+      <c r="M4" s="335"/>
     </row>
     <row r="5" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="284"/>
-      <c r="C5" s="284"/>
-      <c r="D5" s="284"/>
-      <c r="E5" s="284"/>
-      <c r="F5" s="284"/>
-      <c r="G5" s="284"/>
-      <c r="H5" s="284"/>
-      <c r="I5" s="284"/>
-      <c r="J5" s="284"/>
-      <c r="K5" s="284"/>
-      <c r="L5" s="284"/>
-      <c r="M5" s="284"/>
+      <c r="B5" s="320"/>
+      <c r="C5" s="320"/>
+      <c r="D5" s="320"/>
+      <c r="E5" s="320"/>
+      <c r="F5" s="320"/>
+      <c r="G5" s="320"/>
+      <c r="H5" s="320"/>
+      <c r="I5" s="320"/>
+      <c r="J5" s="320"/>
+      <c r="K5" s="320"/>
+      <c r="L5" s="320"/>
+      <c r="M5" s="320"/>
     </row>
     <row r="6" spans="2:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B6" s="12" t="s">
@@ -17881,72 +17881,72 @@
   <sheetData>
     <row r="1" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="285" t="s">
+      <c r="B2" s="321" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="286"/>
-      <c r="D2" s="286"/>
-      <c r="E2" s="286"/>
-      <c r="F2" s="286"/>
-      <c r="G2" s="286"/>
-      <c r="H2" s="286"/>
-      <c r="I2" s="286"/>
-      <c r="J2" s="286"/>
-      <c r="K2" s="286"/>
-      <c r="L2" s="286"/>
-      <c r="M2" s="287"/>
+      <c r="C2" s="322"/>
+      <c r="D2" s="322"/>
+      <c r="E2" s="322"/>
+      <c r="F2" s="322"/>
+      <c r="G2" s="322"/>
+      <c r="H2" s="322"/>
+      <c r="I2" s="322"/>
+      <c r="J2" s="322"/>
+      <c r="K2" s="322"/>
+      <c r="L2" s="322"/>
+      <c r="M2" s="323"/>
     </row>
     <row r="3" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B3" s="288" t="s">
+      <c r="B3" s="324" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="290" t="s">
+      <c r="C3" s="326" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="290" t="s">
+      <c r="D3" s="326" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="292" t="s">
+      <c r="E3" s="328" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="294" t="s">
+      <c r="F3" s="330" t="s">
         <v>1</v>
       </c>
-      <c r="G3" s="295"/>
-      <c r="H3" s="295"/>
-      <c r="I3" s="295"/>
-      <c r="J3" s="295"/>
-      <c r="K3" s="295"/>
-      <c r="L3" s="295"/>
-      <c r="M3" s="296"/>
+      <c r="G3" s="331"/>
+      <c r="H3" s="331"/>
+      <c r="I3" s="331"/>
+      <c r="J3" s="331"/>
+      <c r="K3" s="331"/>
+      <c r="L3" s="331"/>
+      <c r="M3" s="332"/>
     </row>
     <row r="4" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="289"/>
-      <c r="C4" s="291"/>
-      <c r="D4" s="291"/>
-      <c r="E4" s="293"/>
-      <c r="F4" s="297"/>
-      <c r="G4" s="298"/>
-      <c r="H4" s="298"/>
-      <c r="I4" s="298"/>
-      <c r="J4" s="298"/>
-      <c r="K4" s="298"/>
-      <c r="L4" s="298"/>
-      <c r="M4" s="299"/>
+      <c r="B4" s="325"/>
+      <c r="C4" s="327"/>
+      <c r="D4" s="327"/>
+      <c r="E4" s="329"/>
+      <c r="F4" s="333"/>
+      <c r="G4" s="334"/>
+      <c r="H4" s="334"/>
+      <c r="I4" s="334"/>
+      <c r="J4" s="334"/>
+      <c r="K4" s="334"/>
+      <c r="L4" s="334"/>
+      <c r="M4" s="335"/>
     </row>
     <row r="5" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="284"/>
-      <c r="C5" s="284"/>
-      <c r="D5" s="284"/>
-      <c r="E5" s="284"/>
-      <c r="F5" s="300"/>
-      <c r="G5" s="300"/>
-      <c r="H5" s="300"/>
-      <c r="I5" s="300"/>
-      <c r="J5" s="300"/>
-      <c r="K5" s="300"/>
-      <c r="L5" s="300"/>
-      <c r="M5" s="300"/>
+      <c r="B5" s="320"/>
+      <c r="C5" s="320"/>
+      <c r="D5" s="320"/>
+      <c r="E5" s="320"/>
+      <c r="F5" s="336"/>
+      <c r="G5" s="336"/>
+      <c r="H5" s="336"/>
+      <c r="I5" s="336"/>
+      <c r="J5" s="336"/>
+      <c r="K5" s="336"/>
+      <c r="L5" s="336"/>
+      <c r="M5" s="336"/>
     </row>
     <row r="6" spans="2:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B6" s="12" t="s">
@@ -18547,72 +18547,72 @@
   <sheetData>
     <row r="1" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="285" t="s">
+      <c r="B2" s="321" t="s">
         <v>82</v>
       </c>
-      <c r="C2" s="286"/>
-      <c r="D2" s="286"/>
-      <c r="E2" s="286"/>
-      <c r="F2" s="286"/>
-      <c r="G2" s="286"/>
-      <c r="H2" s="286"/>
-      <c r="I2" s="286"/>
-      <c r="J2" s="286"/>
-      <c r="K2" s="286"/>
-      <c r="L2" s="286"/>
-      <c r="M2" s="287"/>
+      <c r="C2" s="322"/>
+      <c r="D2" s="322"/>
+      <c r="E2" s="322"/>
+      <c r="F2" s="322"/>
+      <c r="G2" s="322"/>
+      <c r="H2" s="322"/>
+      <c r="I2" s="322"/>
+      <c r="J2" s="322"/>
+      <c r="K2" s="322"/>
+      <c r="L2" s="322"/>
+      <c r="M2" s="323"/>
     </row>
     <row r="3" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B3" s="288" t="s">
+      <c r="B3" s="324" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="290" t="s">
+      <c r="C3" s="326" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="290" t="s">
+      <c r="D3" s="326" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="292" t="s">
+      <c r="E3" s="328" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="294" t="s">
+      <c r="F3" s="330" t="s">
         <v>84</v>
       </c>
-      <c r="G3" s="295"/>
-      <c r="H3" s="295"/>
-      <c r="I3" s="295"/>
-      <c r="J3" s="295"/>
-      <c r="K3" s="295"/>
-      <c r="L3" s="295"/>
-      <c r="M3" s="296"/>
+      <c r="G3" s="331"/>
+      <c r="H3" s="331"/>
+      <c r="I3" s="331"/>
+      <c r="J3" s="331"/>
+      <c r="K3" s="331"/>
+      <c r="L3" s="331"/>
+      <c r="M3" s="332"/>
     </row>
     <row r="4" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="289"/>
-      <c r="C4" s="291"/>
-      <c r="D4" s="291"/>
-      <c r="E4" s="293"/>
-      <c r="F4" s="297"/>
-      <c r="G4" s="298"/>
-      <c r="H4" s="298"/>
-      <c r="I4" s="298"/>
-      <c r="J4" s="298"/>
-      <c r="K4" s="298"/>
-      <c r="L4" s="298"/>
-      <c r="M4" s="299"/>
+      <c r="B4" s="325"/>
+      <c r="C4" s="327"/>
+      <c r="D4" s="327"/>
+      <c r="E4" s="329"/>
+      <c r="F4" s="333"/>
+      <c r="G4" s="334"/>
+      <c r="H4" s="334"/>
+      <c r="I4" s="334"/>
+      <c r="J4" s="334"/>
+      <c r="K4" s="334"/>
+      <c r="L4" s="334"/>
+      <c r="M4" s="335"/>
     </row>
     <row r="5" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="301"/>
-      <c r="C5" s="284"/>
-      <c r="D5" s="284"/>
-      <c r="E5" s="284"/>
-      <c r="F5" s="284"/>
-      <c r="G5" s="284"/>
-      <c r="H5" s="284"/>
-      <c r="I5" s="284"/>
-      <c r="J5" s="284"/>
-      <c r="K5" s="284"/>
-      <c r="L5" s="284"/>
-      <c r="M5" s="302"/>
+      <c r="B5" s="337"/>
+      <c r="C5" s="320"/>
+      <c r="D5" s="320"/>
+      <c r="E5" s="320"/>
+      <c r="F5" s="320"/>
+      <c r="G5" s="320"/>
+      <c r="H5" s="320"/>
+      <c r="I5" s="320"/>
+      <c r="J5" s="320"/>
+      <c r="K5" s="320"/>
+      <c r="L5" s="320"/>
+      <c r="M5" s="338"/>
     </row>
     <row r="6" spans="2:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B6" s="12" t="s">

</xml_diff>